<commit_message>
Imported new database, working on front-end
</commit_message>
<xml_diff>
--- a/spreadsheets/clips.xlsx
+++ b/spreadsheets/clips.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="2813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3905" uniqueCount="3012">
   <si>
     <t>id</t>
   </si>
@@ -8461,13 +8461,610 @@
   </si>
   <si>
     <t>00;06;30;38</t>
+  </si>
+  <si>
+    <t>help repair</t>
+  </si>
+  <si>
+    <t>00;06;31;23</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>00;06;30;48</t>
+  </si>
+  <si>
+    <t>repair their</t>
+  </si>
+  <si>
+    <t>00;06;31;52</t>
+  </si>
+  <si>
+    <t>their marriage</t>
+  </si>
+  <si>
+    <t>00;06;32;29</t>
+  </si>
+  <si>
+    <t>00;06;31;54</t>
+  </si>
+  <si>
+    <t>planning on</t>
+  </si>
+  <si>
+    <t>00;06;33;55</t>
+  </si>
+  <si>
+    <t>00;06;34;19</t>
+  </si>
+  <si>
+    <t>planning</t>
+  </si>
+  <si>
+    <t>00;06;34;12</t>
+  </si>
+  <si>
+    <t>having</t>
+  </si>
+  <si>
+    <t>00;06;34;18</t>
+  </si>
+  <si>
+    <t>00;06;34;34</t>
+  </si>
+  <si>
+    <t>having a</t>
+  </si>
+  <si>
+    <t>00;06;34;41</t>
+  </si>
+  <si>
+    <t>at the top</t>
+  </si>
+  <si>
+    <t>00;06;35;02</t>
+  </si>
+  <si>
+    <t>00;06;35;26</t>
+  </si>
+  <si>
+    <t>the top</t>
+  </si>
+  <si>
+    <t>00;06;35;07</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>00;06;35;14</t>
+  </si>
+  <si>
+    <t>00;06;35;28</t>
+  </si>
+  <si>
+    <t>the hill</t>
+  </si>
+  <si>
+    <t>00;06;35;29</t>
+  </si>
+  <si>
+    <t>00;06;35;51</t>
+  </si>
+  <si>
+    <t>hill</t>
+  </si>
+  <si>
+    <t>00;06;35;35</t>
+  </si>
+  <si>
+    <t>payoff</t>
+  </si>
+  <si>
+    <t>00;06;41;27</t>
+  </si>
+  <si>
+    <t>00;06;41;54</t>
+  </si>
+  <si>
+    <t>pay</t>
+  </si>
+  <si>
+    <t>00;06;41;43</t>
+  </si>
+  <si>
+    <t>arduous</t>
+  </si>
+  <si>
+    <t>00;06;42;20</t>
+  </si>
+  <si>
+    <t>00;06;42;50</t>
+  </si>
+  <si>
+    <t>one hour</t>
+  </si>
+  <si>
+    <t>00;06;42;52</t>
+  </si>
+  <si>
+    <t>00;06;43;14</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>00;06;43;03</t>
+  </si>
+  <si>
+    <t>trek</t>
+  </si>
+  <si>
+    <t>00;06;43;15</t>
+  </si>
+  <si>
+    <t>00;06;43;32</t>
+  </si>
+  <si>
+    <t>woods</t>
+  </si>
+  <si>
+    <t>00;06;43;48</t>
+  </si>
+  <si>
+    <t>00;06;44;14</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>00;06;44;04</t>
+  </si>
+  <si>
+    <t>would</t>
+  </si>
+  <si>
+    <t>is this</t>
+  </si>
+  <si>
+    <t>00;06;44;05</t>
+  </si>
+  <si>
+    <t>00;06;44;52</t>
+  </si>
+  <si>
+    <t>00;06;44;28</t>
+  </si>
+  <si>
+    <t>00;06;44;29</t>
+  </si>
+  <si>
+    <t>00;06;44;58</t>
+  </si>
+  <si>
+    <t>00;06;44;59</t>
+  </si>
+  <si>
+    <t>00;06;46;01</t>
+  </si>
+  <si>
+    <t>a panoramic view</t>
+  </si>
+  <si>
+    <t>00;06;46;20</t>
+  </si>
+  <si>
+    <t>a panoramic</t>
+  </si>
+  <si>
+    <t>panoramic</t>
+  </si>
+  <si>
+    <t>00;06;45;23</t>
+  </si>
+  <si>
+    <t>00;06;46;00</t>
+  </si>
+  <si>
+    <t>panoramic view</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>00;06;46;30</t>
+  </si>
+  <si>
+    <t>00;06;46;45</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>00;06;50;15</t>
+  </si>
+  <si>
+    <t>00;06;50;33</t>
+  </si>
+  <si>
+    <t>went through</t>
+  </si>
+  <si>
+    <t>00;06;50;34</t>
+  </si>
+  <si>
+    <t>00;06;51;07</t>
+  </si>
+  <si>
+    <t>00;06;50;49</t>
+  </si>
+  <si>
+    <t>through my</t>
+  </si>
+  <si>
+    <t>00;06;51;20</t>
+  </si>
+  <si>
+    <t>my mind</t>
+  </si>
+  <si>
+    <t>00;06;51;09</t>
+  </si>
+  <si>
+    <t>00;06;51;56</t>
+  </si>
+  <si>
+    <t>mind</t>
+  </si>
+  <si>
+    <t>00;06;51;19</t>
+  </si>
+  <si>
+    <t>mind was</t>
+  </si>
+  <si>
+    <t>00;06;52;41</t>
+  </si>
+  <si>
+    <t>my mind was</t>
+  </si>
+  <si>
+    <t>00;06;52;03</t>
+  </si>
+  <si>
+    <t>00;06;52;56</t>
+  </si>
+  <si>
+    <t>00;06;53;17</t>
+  </si>
+  <si>
+    <t>i have</t>
+  </si>
+  <si>
+    <t>00;06;53;06</t>
+  </si>
+  <si>
+    <t>00;06;53;26</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>00;06;54;02</t>
+  </si>
+  <si>
+    <t>00;06;54;31</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>00;06;54;24</t>
+  </si>
+  <si>
+    <t>to live</t>
+  </si>
+  <si>
+    <t>00;06;54;27</t>
+  </si>
+  <si>
+    <t>00;06;55;07</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
+  <si>
+    <t>00;06;54;40</t>
+  </si>
+  <si>
+    <t>it is</t>
+  </si>
+  <si>
+    <t>00;06;55;09</t>
+  </si>
+  <si>
+    <t>00;06;55;29</t>
+  </si>
+  <si>
+    <t>is here</t>
+  </si>
+  <si>
+    <t>00;06;55;17</t>
+  </si>
+  <si>
+    <t>00;06;55;45</t>
+  </si>
+  <si>
+    <t>00;06;55;24</t>
+  </si>
+  <si>
+    <t>hear that</t>
+  </si>
+  <si>
+    <t>00;06;55;55</t>
+  </si>
+  <si>
+    <t>here that</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>00;06;56;19</t>
+  </si>
+  <si>
+    <t>00;06;56;39</t>
+  </si>
+  <si>
+    <t>tried to kill</t>
+  </si>
+  <si>
+    <t>00;06;56;35</t>
+  </si>
+  <si>
+    <t>00;06;57;20</t>
+  </si>
+  <si>
+    <t>tried to</t>
+  </si>
+  <si>
+    <t>00;06;57;04</t>
+  </si>
+  <si>
+    <t>tried</t>
+  </si>
+  <si>
+    <t>00;06;56;55</t>
+  </si>
+  <si>
+    <t>to kill</t>
+  </si>
+  <si>
+    <t>00;06;56;56</t>
+  </si>
+  <si>
+    <t>00;06;57;21</t>
+  </si>
+  <si>
+    <t>00;06;57;06</t>
+  </si>
+  <si>
+    <t>00;06;57;57</t>
+  </si>
+  <si>
+    <t>kill his wife</t>
+  </si>
+  <si>
+    <t>kill his</t>
+  </si>
+  <si>
+    <t>00;06;57;31</t>
+  </si>
+  <si>
+    <t>his</t>
+  </si>
+  <si>
+    <t>00;06;57;32</t>
+  </si>
+  <si>
+    <t>00;06;58;00</t>
+  </si>
+  <si>
+    <t>his wife</t>
+  </si>
+  <si>
+    <t>00;06;58;01</t>
+  </si>
+  <si>
+    <t>00;06;58;28</t>
+  </si>
+  <si>
+    <t>he bashed</t>
+  </si>
+  <si>
+    <t>00;06;58;51</t>
+  </si>
+  <si>
+    <t>bashed</t>
+  </si>
+  <si>
+    <t>00;06;58;26</t>
+  </si>
+  <si>
+    <t>in the back</t>
+  </si>
+  <si>
+    <t>00;06;59;12</t>
+  </si>
+  <si>
+    <t>00;06;59;37</t>
+  </si>
+  <si>
+    <t>00;06;59;19</t>
+  </si>
+  <si>
+    <t>back of</t>
+  </si>
+  <si>
+    <t>00;06;59;40</t>
+  </si>
+  <si>
+    <t>the back</t>
+  </si>
+  <si>
+    <t>00;06;59;35</t>
+  </si>
+  <si>
+    <t>the head</t>
+  </si>
+  <si>
+    <t>00;06;59;38</t>
+  </si>
+  <si>
+    <t>00;07;00;07</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>00;06;59;45</t>
+  </si>
+  <si>
+    <t>with a rock</t>
+  </si>
+  <si>
+    <t>00;07;00;08</t>
+  </si>
+  <si>
+    <t>00;07;00;43</t>
+  </si>
+  <si>
+    <t>with iraq</t>
+  </si>
+  <si>
+    <t>iraq</t>
+  </si>
+  <si>
+    <t>00;07;00;15</t>
+  </si>
+  <si>
+    <t>a rock</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>00;07;00;19</t>
+  </si>
+  <si>
+    <t>00;07;00;44</t>
+  </si>
+  <si>
+    <t>00;07;01;13</t>
+  </si>
+  <si>
+    <t>and pushed</t>
+  </si>
+  <si>
+    <t>00;07;01;35</t>
+  </si>
+  <si>
+    <t>and push</t>
+  </si>
+  <si>
+    <t>00;07;01;44</t>
+  </si>
+  <si>
+    <t>00;07;01;59</t>
+  </si>
+  <si>
+    <t>down this</t>
+  </si>
+  <si>
+    <t>00;07;02;11</t>
+  </si>
+  <si>
+    <t>eight hundred</t>
+  </si>
+  <si>
+    <t>00;07;02;12</t>
+  </si>
+  <si>
+    <t>00;07;03;05</t>
+  </si>
+  <si>
+    <t>00;07;02;35</t>
+  </si>
+  <si>
+    <t>hundred</t>
+  </si>
+  <si>
+    <t>00;07;02;36</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>00;07;03;06</t>
+  </si>
+  <si>
+    <t>00;07;03;25</t>
+  </si>
+  <si>
+    <t>hundred foot</t>
+  </si>
+  <si>
+    <t>00;07;03;26</t>
+  </si>
+  <si>
+    <t>00;07;03;57</t>
+  </si>
+  <si>
+    <t>the story</t>
+  </si>
+  <si>
+    <t>00;07;04;15</t>
+  </si>
+  <si>
+    <t>00;07;04;57</t>
+  </si>
+  <si>
+    <t>00;07;04;28</t>
+  </si>
+  <si>
+    <t>00;07;04;29</t>
+  </si>
+  <si>
+    <t>story of how</t>
+  </si>
+  <si>
+    <t>00;07;05;15</t>
+  </si>
+  <si>
+    <t>how</t>
+  </si>
+  <si>
+    <t>00;07;05;00</t>
+  </si>
+  <si>
+    <t>how she</t>
+  </si>
+  <si>
+    <t>00;07;05;27</t>
+  </si>
+  <si>
+    <t>00;07;05;18</t>
+  </si>
+  <si>
+    <t>00;07;05;31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8494,6 +9091,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -8512,7 +9117,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8684,12 +9289,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -8775,6 +9431,31 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -8860,6 +9541,31 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9189,10 +9895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1250"/>
+  <dimension ref="A1:H1300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1194" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F1201" sqref="F1201"/>
+    <sheetView tabSelected="1" topLeftCell="A1286" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F1300" sqref="F1300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40441,6 +41147,15 @@
       <c r="C1202">
         <v>4</v>
       </c>
+      <c r="D1202" t="s">
+        <v>2813</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>2812</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>2814</v>
+      </c>
       <c r="G1202">
         <v>0</v>
       </c>
@@ -40458,6 +41173,15 @@
       <c r="C1203">
         <v>4</v>
       </c>
+      <c r="D1203" t="s">
+        <v>2815</v>
+      </c>
+      <c r="E1203" t="s">
+        <v>2816</v>
+      </c>
+      <c r="F1203" t="s">
+        <v>2814</v>
+      </c>
       <c r="G1203">
         <v>0</v>
       </c>
@@ -40475,6 +41199,15 @@
       <c r="C1204">
         <v>4</v>
       </c>
+      <c r="D1204" t="s">
+        <v>2817</v>
+      </c>
+      <c r="E1204" t="s">
+        <v>2816</v>
+      </c>
+      <c r="F1204" t="s">
+        <v>2818</v>
+      </c>
       <c r="G1204">
         <v>0</v>
       </c>
@@ -40492,6 +41225,15 @@
       <c r="C1205">
         <v>4</v>
       </c>
+      <c r="D1205" t="s">
+        <v>2819</v>
+      </c>
+      <c r="E1205" t="s">
+        <v>2814</v>
+      </c>
+      <c r="F1205" t="s">
+        <v>2820</v>
+      </c>
       <c r="G1205">
         <v>0</v>
       </c>
@@ -40509,6 +41251,15 @@
       <c r="C1206">
         <v>4</v>
       </c>
+      <c r="D1206" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1206" t="s">
+        <v>2814</v>
+      </c>
+      <c r="F1206" t="s">
+        <v>2821</v>
+      </c>
       <c r="G1206">
         <v>0</v>
       </c>
@@ -40526,6 +41277,15 @@
       <c r="C1207">
         <v>4</v>
       </c>
+      <c r="D1207" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1207" t="s">
+        <v>2814</v>
+      </c>
+      <c r="F1207" t="s">
+        <v>2821</v>
+      </c>
       <c r="G1207">
         <v>0</v>
       </c>
@@ -40543,6 +41303,15 @@
       <c r="C1208">
         <v>4</v>
       </c>
+      <c r="D1208" t="s">
+        <v>2822</v>
+      </c>
+      <c r="E1208" t="s">
+        <v>2823</v>
+      </c>
+      <c r="F1208" t="s">
+        <v>2824</v>
+      </c>
       <c r="G1208">
         <v>0</v>
       </c>
@@ -40560,6 +41329,15 @@
       <c r="C1209">
         <v>4</v>
       </c>
+      <c r="D1209" t="s">
+        <v>2825</v>
+      </c>
+      <c r="E1209" t="s">
+        <v>2823</v>
+      </c>
+      <c r="F1209" t="s">
+        <v>2826</v>
+      </c>
       <c r="G1209">
         <v>0</v>
       </c>
@@ -40577,6 +41355,15 @@
       <c r="C1210">
         <v>4</v>
       </c>
+      <c r="D1210" t="s">
+        <v>2827</v>
+      </c>
+      <c r="E1210" t="s">
+        <v>2828</v>
+      </c>
+      <c r="F1210" t="s">
+        <v>2829</v>
+      </c>
       <c r="G1210">
         <v>0</v>
       </c>
@@ -40594,6 +41381,15 @@
       <c r="C1211">
         <v>4</v>
       </c>
+      <c r="D1211" t="s">
+        <v>2830</v>
+      </c>
+      <c r="E1211" t="s">
+        <v>2828</v>
+      </c>
+      <c r="F1211" t="s">
+        <v>2831</v>
+      </c>
       <c r="G1211">
         <v>0</v>
       </c>
@@ -40611,6 +41407,15 @@
       <c r="C1212">
         <v>4</v>
       </c>
+      <c r="D1212" t="s">
+        <v>2832</v>
+      </c>
+      <c r="E1212" t="s">
+        <v>2833</v>
+      </c>
+      <c r="F1212" t="s">
+        <v>2834</v>
+      </c>
       <c r="G1212">
         <v>0</v>
       </c>
@@ -40628,6 +41433,15 @@
       <c r="C1213">
         <v>4</v>
       </c>
+      <c r="D1213" t="s">
+        <v>2835</v>
+      </c>
+      <c r="E1213" t="s">
+        <v>2836</v>
+      </c>
+      <c r="F1213" t="s">
+        <v>2834</v>
+      </c>
       <c r="G1213">
         <v>0</v>
       </c>
@@ -40645,6 +41459,15 @@
       <c r="C1214">
         <v>4</v>
       </c>
+      <c r="D1214" t="s">
+        <v>2837</v>
+      </c>
+      <c r="E1214" t="s">
+        <v>2838</v>
+      </c>
+      <c r="F1214" t="s">
+        <v>2839</v>
+      </c>
       <c r="G1214">
         <v>0</v>
       </c>
@@ -40662,6 +41485,15 @@
       <c r="C1215">
         <v>4</v>
       </c>
+      <c r="D1215" t="s">
+        <v>2840</v>
+      </c>
+      <c r="E1215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="F1215" t="s">
+        <v>2842</v>
+      </c>
       <c r="G1215">
         <v>0</v>
       </c>
@@ -40679,6 +41511,15 @@
       <c r="C1216">
         <v>4</v>
       </c>
+      <c r="D1216" t="s">
+        <v>2843</v>
+      </c>
+      <c r="E1216" t="s">
+        <v>2844</v>
+      </c>
+      <c r="F1216" t="s">
+        <v>2842</v>
+      </c>
       <c r="G1216">
         <v>0</v>
       </c>
@@ -40696,6 +41537,15 @@
       <c r="C1217">
         <v>4</v>
       </c>
+      <c r="D1217" t="s">
+        <v>2845</v>
+      </c>
+      <c r="E1217" t="s">
+        <v>2846</v>
+      </c>
+      <c r="F1217" t="s">
+        <v>2847</v>
+      </c>
       <c r="G1217">
         <v>0</v>
       </c>
@@ -40713,6 +41563,15 @@
       <c r="C1218">
         <v>4</v>
       </c>
+      <c r="D1218" t="s">
+        <v>2848</v>
+      </c>
+      <c r="E1218" t="s">
+        <v>2846</v>
+      </c>
+      <c r="F1218" t="s">
+        <v>2849</v>
+      </c>
       <c r="G1218">
         <v>0</v>
       </c>
@@ -40730,6 +41589,15 @@
       <c r="C1219">
         <v>4</v>
       </c>
+      <c r="D1219" t="s">
+        <v>2850</v>
+      </c>
+      <c r="E1219" t="s">
+        <v>2851</v>
+      </c>
+      <c r="F1219" t="s">
+        <v>2852</v>
+      </c>
       <c r="G1219">
         <v>0</v>
       </c>
@@ -40747,6 +41615,15 @@
       <c r="C1220">
         <v>4</v>
       </c>
+      <c r="D1220" t="s">
+        <v>2853</v>
+      </c>
+      <c r="E1220" t="s">
+        <v>2854</v>
+      </c>
+      <c r="F1220" t="s">
+        <v>2855</v>
+      </c>
       <c r="G1220">
         <v>0</v>
       </c>
@@ -40764,6 +41641,15 @@
       <c r="C1221">
         <v>4</v>
       </c>
+      <c r="D1221" t="s">
+        <v>2856</v>
+      </c>
+      <c r="E1221" t="s">
+        <v>2857</v>
+      </c>
+      <c r="F1221" t="s">
+        <v>2855</v>
+      </c>
       <c r="G1221">
         <v>0</v>
       </c>
@@ -40781,6 +41667,15 @@
       <c r="C1222">
         <v>4</v>
       </c>
+      <c r="D1222" t="s">
+        <v>2858</v>
+      </c>
+      <c r="E1222" t="s">
+        <v>2859</v>
+      </c>
+      <c r="F1222" t="s">
+        <v>2860</v>
+      </c>
       <c r="G1222">
         <v>0</v>
       </c>
@@ -40798,6 +41693,15 @@
       <c r="C1223">
         <v>4</v>
       </c>
+      <c r="D1223" t="s">
+        <v>2861</v>
+      </c>
+      <c r="E1223" t="s">
+        <v>2862</v>
+      </c>
+      <c r="F1223" t="s">
+        <v>2863</v>
+      </c>
       <c r="G1223">
         <v>0</v>
       </c>
@@ -40815,6 +41719,15 @@
       <c r="C1224">
         <v>4</v>
       </c>
+      <c r="D1224" t="s">
+        <v>2864</v>
+      </c>
+      <c r="E1224" t="s">
+        <v>2862</v>
+      </c>
+      <c r="F1224" t="s">
+        <v>2865</v>
+      </c>
       <c r="G1224">
         <v>0</v>
       </c>
@@ -40832,6 +41745,15 @@
       <c r="C1225">
         <v>4</v>
       </c>
+      <c r="D1225" t="s">
+        <v>2866</v>
+      </c>
+      <c r="E1225" t="s">
+        <v>2862</v>
+      </c>
+      <c r="F1225" t="s">
+        <v>2865</v>
+      </c>
       <c r="G1225">
         <v>0</v>
       </c>
@@ -40849,6 +41771,15 @@
       <c r="C1226">
         <v>4</v>
       </c>
+      <c r="D1226" t="s">
+        <v>2867</v>
+      </c>
+      <c r="E1226" t="s">
+        <v>2868</v>
+      </c>
+      <c r="F1226" t="s">
+        <v>2869</v>
+      </c>
       <c r="G1226">
         <v>0</v>
       </c>
@@ -40866,6 +41797,15 @@
       <c r="C1227">
         <v>4</v>
       </c>
+      <c r="D1227" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1227" t="s">
+        <v>2868</v>
+      </c>
+      <c r="F1227" t="s">
+        <v>2870</v>
+      </c>
       <c r="G1227">
         <v>0</v>
       </c>
@@ -40883,6 +41823,15 @@
       <c r="C1228">
         <v>4</v>
       </c>
+      <c r="D1228" t="s">
+        <v>474</v>
+      </c>
+      <c r="E1228" t="s">
+        <v>2871</v>
+      </c>
+      <c r="F1228" t="s">
+        <v>2872</v>
+      </c>
       <c r="G1228">
         <v>0</v>
       </c>
@@ -40900,6 +41849,15 @@
       <c r="C1229">
         <v>4</v>
       </c>
+      <c r="D1229" t="s">
+        <v>2877</v>
+      </c>
+      <c r="E1229" t="s">
+        <v>2873</v>
+      </c>
+      <c r="F1229" t="s">
+        <v>2874</v>
+      </c>
       <c r="G1229">
         <v>0</v>
       </c>
@@ -40917,6 +41875,15 @@
       <c r="C1230">
         <v>4</v>
       </c>
+      <c r="D1230" t="s">
+        <v>2875</v>
+      </c>
+      <c r="E1230" t="s">
+        <v>2873</v>
+      </c>
+      <c r="F1230" t="s">
+        <v>2876</v>
+      </c>
       <c r="G1230">
         <v>0</v>
       </c>
@@ -40934,6 +41901,15 @@
       <c r="C1231">
         <v>4</v>
       </c>
+      <c r="D1231" t="s">
+        <v>2878</v>
+      </c>
+      <c r="E1231" t="s">
+        <v>2879</v>
+      </c>
+      <c r="F1231" t="s">
+        <v>2880</v>
+      </c>
       <c r="G1231">
         <v>0</v>
       </c>
@@ -40951,6 +41927,15 @@
       <c r="C1232">
         <v>4</v>
       </c>
+      <c r="D1232" t="s">
+        <v>2881</v>
+      </c>
+      <c r="E1232" t="s">
+        <v>2879</v>
+      </c>
+      <c r="F1232" t="s">
+        <v>2876</v>
+      </c>
       <c r="G1232">
         <v>0</v>
       </c>
@@ -40968,6 +41953,15 @@
       <c r="C1233">
         <v>4</v>
       </c>
+      <c r="D1233" t="s">
+        <v>2882</v>
+      </c>
+      <c r="E1233" t="s">
+        <v>2874</v>
+      </c>
+      <c r="F1233" t="s">
+        <v>2876</v>
+      </c>
       <c r="G1233">
         <v>0</v>
       </c>
@@ -40985,6 +41979,15 @@
       <c r="C1234">
         <v>4</v>
       </c>
+      <c r="D1234" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E1234" t="s">
+        <v>2883</v>
+      </c>
+      <c r="F1234" t="s">
+        <v>2884</v>
+      </c>
       <c r="G1234">
         <v>0</v>
       </c>
@@ -41002,6 +42005,15 @@
       <c r="C1235">
         <v>4</v>
       </c>
+      <c r="D1235" t="s">
+        <v>2885</v>
+      </c>
+      <c r="E1235" t="s">
+        <v>2886</v>
+      </c>
+      <c r="F1235" t="s">
+        <v>2887</v>
+      </c>
       <c r="G1235">
         <v>0</v>
       </c>
@@ -41019,6 +42031,15 @@
       <c r="C1236">
         <v>4</v>
       </c>
+      <c r="D1236" t="s">
+        <v>2888</v>
+      </c>
+      <c r="E1236" t="s">
+        <v>2889</v>
+      </c>
+      <c r="F1236" t="s">
+        <v>2890</v>
+      </c>
       <c r="G1236">
         <v>0</v>
       </c>
@@ -41036,6 +42057,15 @@
       <c r="C1237">
         <v>4</v>
       </c>
+      <c r="D1237" t="s">
+        <v>464</v>
+      </c>
+      <c r="E1237" t="s">
+        <v>2889</v>
+      </c>
+      <c r="F1237" t="s">
+        <v>2891</v>
+      </c>
       <c r="G1237">
         <v>0</v>
       </c>
@@ -41053,6 +42083,15 @@
       <c r="C1238">
         <v>4</v>
       </c>
+      <c r="D1238" t="s">
+        <v>832</v>
+      </c>
+      <c r="E1238" t="s">
+        <v>2891</v>
+      </c>
+      <c r="F1238" t="s">
+        <v>2890</v>
+      </c>
       <c r="G1238">
         <v>0</v>
       </c>
@@ -41070,6 +42109,15 @@
       <c r="C1239">
         <v>4</v>
       </c>
+      <c r="D1239" t="s">
+        <v>2892</v>
+      </c>
+      <c r="E1239" t="s">
+        <v>2891</v>
+      </c>
+      <c r="F1239" t="s">
+        <v>2893</v>
+      </c>
       <c r="G1239">
         <v>0</v>
       </c>
@@ -41087,6 +42135,15 @@
       <c r="C1240">
         <v>4</v>
       </c>
+      <c r="D1240" t="s">
+        <v>2894</v>
+      </c>
+      <c r="E1240" t="s">
+        <v>2895</v>
+      </c>
+      <c r="F1240" t="s">
+        <v>2896</v>
+      </c>
       <c r="G1240">
         <v>0</v>
       </c>
@@ -41104,6 +42161,15 @@
       <c r="C1241">
         <v>4</v>
       </c>
+      <c r="D1241" t="s">
+        <v>2897</v>
+      </c>
+      <c r="E1241" t="s">
+        <v>2898</v>
+      </c>
+      <c r="F1241" t="s">
+        <v>2896</v>
+      </c>
       <c r="G1241">
         <v>0</v>
       </c>
@@ -41121,6 +42187,15 @@
       <c r="C1242">
         <v>4</v>
       </c>
+      <c r="D1242" t="s">
+        <v>2899</v>
+      </c>
+      <c r="E1242" t="s">
+        <v>2898</v>
+      </c>
+      <c r="F1242" t="s">
+        <v>2900</v>
+      </c>
       <c r="G1242">
         <v>0</v>
       </c>
@@ -41138,6 +42213,15 @@
       <c r="C1243">
         <v>4</v>
       </c>
+      <c r="D1243" t="s">
+        <v>2901</v>
+      </c>
+      <c r="E1243" t="s">
+        <v>2895</v>
+      </c>
+      <c r="F1243" t="s">
+        <v>2900</v>
+      </c>
       <c r="G1243">
         <v>0</v>
       </c>
@@ -41155,6 +42239,15 @@
       <c r="C1244">
         <v>4</v>
       </c>
+      <c r="D1244" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1244" t="s">
+        <v>2902</v>
+      </c>
+      <c r="F1244" t="s">
+        <v>2900</v>
+      </c>
       <c r="G1244">
         <v>0</v>
       </c>
@@ -41172,6 +42265,15 @@
       <c r="C1245">
         <v>4</v>
       </c>
+      <c r="D1245" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1245" t="s">
+        <v>2903</v>
+      </c>
+      <c r="F1245" t="s">
+        <v>2904</v>
+      </c>
       <c r="G1245">
         <v>0</v>
       </c>
@@ -41189,6 +42291,15 @@
       <c r="C1246">
         <v>4</v>
       </c>
+      <c r="D1246" t="s">
+        <v>2905</v>
+      </c>
+      <c r="E1246" t="s">
+        <v>2906</v>
+      </c>
+      <c r="F1246" t="s">
+        <v>2907</v>
+      </c>
       <c r="G1246">
         <v>0</v>
       </c>
@@ -41206,6 +42317,15 @@
       <c r="C1247">
         <v>4</v>
       </c>
+      <c r="D1247" t="s">
+        <v>2908</v>
+      </c>
+      <c r="E1247" t="s">
+        <v>2909</v>
+      </c>
+      <c r="F1247" t="s">
+        <v>2910</v>
+      </c>
       <c r="G1247">
         <v>0</v>
       </c>
@@ -41223,6 +42343,15 @@
       <c r="C1248">
         <v>4</v>
       </c>
+      <c r="D1248" t="s">
+        <v>2911</v>
+      </c>
+      <c r="E1248" t="s">
+        <v>2909</v>
+      </c>
+      <c r="F1248" t="s">
+        <v>2912</v>
+      </c>
       <c r="G1248">
         <v>0</v>
       </c>
@@ -41240,6 +42369,15 @@
       <c r="C1249">
         <v>4</v>
       </c>
+      <c r="D1249" t="s">
+        <v>2913</v>
+      </c>
+      <c r="E1249" t="s">
+        <v>2914</v>
+      </c>
+      <c r="F1249" t="s">
+        <v>2915</v>
+      </c>
       <c r="G1249">
         <v>0</v>
       </c>
@@ -41257,10 +42395,1319 @@
       <c r="C1250">
         <v>4</v>
       </c>
+      <c r="D1250" t="s">
+        <v>2916</v>
+      </c>
+      <c r="E1250" t="s">
+        <v>2917</v>
+      </c>
+      <c r="F1250" t="s">
+        <v>2915</v>
+      </c>
       <c r="G1250">
         <v>0</v>
       </c>
       <c r="H1250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:8">
+      <c r="A1251">
+        <v>1250</v>
+      </c>
+      <c r="B1251">
+        <v>3</v>
+      </c>
+      <c r="C1251">
+        <v>4</v>
+      </c>
+      <c r="D1251" t="s">
+        <v>2918</v>
+      </c>
+      <c r="E1251" t="s">
+        <v>2919</v>
+      </c>
+      <c r="F1251" t="s">
+        <v>2920</v>
+      </c>
+      <c r="G1251">
+        <v>0</v>
+      </c>
+      <c r="H1251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:8">
+      <c r="A1252">
+        <v>1251</v>
+      </c>
+      <c r="B1252">
+        <v>3</v>
+      </c>
+      <c r="C1252">
+        <v>4</v>
+      </c>
+      <c r="D1252" t="s">
+        <v>2921</v>
+      </c>
+      <c r="E1252" t="s">
+        <v>2922</v>
+      </c>
+      <c r="F1252" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G1252">
+        <v>0</v>
+      </c>
+      <c r="H1252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:8">
+      <c r="A1253">
+        <v>1252</v>
+      </c>
+      <c r="B1253">
+        <v>3</v>
+      </c>
+      <c r="C1253">
+        <v>4</v>
+      </c>
+      <c r="D1253" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1253" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1253" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G1253">
+        <v>0</v>
+      </c>
+      <c r="H1253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:8">
+      <c r="A1254">
+        <v>1253</v>
+      </c>
+      <c r="B1254">
+        <v>3</v>
+      </c>
+      <c r="C1254">
+        <v>4</v>
+      </c>
+      <c r="D1254" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1254" t="s">
+        <v>2923</v>
+      </c>
+      <c r="G1254">
+        <v>0</v>
+      </c>
+      <c r="H1254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:8">
+      <c r="A1255">
+        <v>1254</v>
+      </c>
+      <c r="B1255">
+        <v>3</v>
+      </c>
+      <c r="C1255">
+        <v>4</v>
+      </c>
+      <c r="D1255" t="s">
+        <v>2925</v>
+      </c>
+      <c r="E1255" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1255" t="s">
+        <v>2926</v>
+      </c>
+      <c r="G1255">
+        <v>0</v>
+      </c>
+      <c r="H1255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:8">
+      <c r="A1256">
+        <v>1255</v>
+      </c>
+      <c r="B1256">
+        <v>3</v>
+      </c>
+      <c r="C1256">
+        <v>4</v>
+      </c>
+      <c r="D1256" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E1256" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F1256" t="s">
+        <v>2926</v>
+      </c>
+      <c r="G1256">
+        <v>0</v>
+      </c>
+      <c r="H1256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:8">
+      <c r="A1257">
+        <v>1256</v>
+      </c>
+      <c r="B1257">
+        <v>3</v>
+      </c>
+      <c r="C1257">
+        <v>4</v>
+      </c>
+      <c r="D1257" t="s">
+        <v>2928</v>
+      </c>
+      <c r="E1257" t="s">
+        <v>2929</v>
+      </c>
+      <c r="F1257" t="s">
+        <v>2930</v>
+      </c>
+      <c r="G1257">
+        <v>0</v>
+      </c>
+      <c r="H1257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:8">
+      <c r="A1258">
+        <v>1257</v>
+      </c>
+      <c r="B1258">
+        <v>3</v>
+      </c>
+      <c r="C1258">
+        <v>4</v>
+      </c>
+      <c r="D1258" t="s">
+        <v>2931</v>
+      </c>
+      <c r="E1258" t="s">
+        <v>2932</v>
+      </c>
+      <c r="F1258" t="s">
+        <v>2933</v>
+      </c>
+      <c r="G1258">
+        <v>0</v>
+      </c>
+      <c r="H1258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:8">
+      <c r="A1259">
+        <v>1258</v>
+      </c>
+      <c r="B1259">
+        <v>3</v>
+      </c>
+      <c r="C1259">
+        <v>4</v>
+      </c>
+      <c r="D1259" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E1259" t="s">
+        <v>2932</v>
+      </c>
+      <c r="F1259" t="s">
+        <v>2935</v>
+      </c>
+      <c r="G1259">
+        <v>0</v>
+      </c>
+      <c r="H1259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:8">
+      <c r="A1260">
+        <v>1259</v>
+      </c>
+      <c r="B1260">
+        <v>3</v>
+      </c>
+      <c r="C1260">
+        <v>4</v>
+      </c>
+      <c r="D1260" t="s">
+        <v>2936</v>
+      </c>
+      <c r="E1260" t="s">
+        <v>2932</v>
+      </c>
+      <c r="F1260" t="s">
+        <v>2937</v>
+      </c>
+      <c r="G1260">
+        <v>0</v>
+      </c>
+      <c r="H1260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:8">
+      <c r="A1261">
+        <v>1260</v>
+      </c>
+      <c r="B1261">
+        <v>3</v>
+      </c>
+      <c r="C1261">
+        <v>4</v>
+      </c>
+      <c r="D1261" t="s">
+        <v>2938</v>
+      </c>
+      <c r="E1261" t="s">
+        <v>2939</v>
+      </c>
+      <c r="F1261" t="s">
+        <v>2940</v>
+      </c>
+      <c r="G1261">
+        <v>0</v>
+      </c>
+      <c r="H1261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:8">
+      <c r="A1262">
+        <v>1261</v>
+      </c>
+      <c r="B1262">
+        <v>3</v>
+      </c>
+      <c r="C1262">
+        <v>4</v>
+      </c>
+      <c r="D1262" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E1262" t="s">
+        <v>2941</v>
+      </c>
+      <c r="F1262" t="s">
+        <v>2940</v>
+      </c>
+      <c r="G1262">
+        <v>0</v>
+      </c>
+      <c r="H1262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:8">
+      <c r="A1263">
+        <v>1262</v>
+      </c>
+      <c r="B1263">
+        <v>3</v>
+      </c>
+      <c r="C1263">
+        <v>4</v>
+      </c>
+      <c r="D1263" t="s">
+        <v>2943</v>
+      </c>
+      <c r="E1263" t="s">
+        <v>2941</v>
+      </c>
+      <c r="F1263" t="s">
+        <v>2942</v>
+      </c>
+      <c r="G1263">
+        <v>0</v>
+      </c>
+      <c r="H1263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:8">
+      <c r="A1264">
+        <v>1263</v>
+      </c>
+      <c r="B1264">
+        <v>3</v>
+      </c>
+      <c r="C1264">
+        <v>4</v>
+      </c>
+      <c r="D1264" t="s">
+        <v>2944</v>
+      </c>
+      <c r="E1264" t="s">
+        <v>2941</v>
+      </c>
+      <c r="F1264" t="s">
+        <v>2945</v>
+      </c>
+      <c r="G1264">
+        <v>0</v>
+      </c>
+      <c r="H1264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:8">
+      <c r="A1265">
+        <v>1264</v>
+      </c>
+      <c r="B1265">
+        <v>3</v>
+      </c>
+      <c r="C1265">
+        <v>4</v>
+      </c>
+      <c r="D1265" t="s">
+        <v>2946</v>
+      </c>
+      <c r="E1265" t="s">
+        <v>2940</v>
+      </c>
+      <c r="F1265" t="s">
+        <v>2945</v>
+      </c>
+      <c r="G1265">
+        <v>0</v>
+      </c>
+      <c r="H1265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:8">
+      <c r="A1266">
+        <v>1265</v>
+      </c>
+      <c r="B1266">
+        <v>3</v>
+      </c>
+      <c r="C1266">
+        <v>4</v>
+      </c>
+      <c r="D1266" t="s">
+        <v>2574</v>
+      </c>
+      <c r="E1266" t="s">
+        <v>2947</v>
+      </c>
+      <c r="F1266" t="s">
+        <v>2948</v>
+      </c>
+      <c r="G1266">
+        <v>0</v>
+      </c>
+      <c r="H1266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:8">
+      <c r="A1267">
+        <v>1266</v>
+      </c>
+      <c r="B1267">
+        <v>3</v>
+      </c>
+      <c r="C1267">
+        <v>4</v>
+      </c>
+      <c r="D1267" t="s">
+        <v>2949</v>
+      </c>
+      <c r="E1267" t="s">
+        <v>2940</v>
+      </c>
+      <c r="F1267" t="s">
+        <v>2948</v>
+      </c>
+      <c r="G1267">
+        <v>0</v>
+      </c>
+      <c r="H1267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:8">
+      <c r="A1268">
+        <v>1267</v>
+      </c>
+      <c r="B1268">
+        <v>3</v>
+      </c>
+      <c r="C1268">
+        <v>4</v>
+      </c>
+      <c r="D1268" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1268" t="s">
+        <v>2950</v>
+      </c>
+      <c r="F1268" t="s">
+        <v>2951</v>
+      </c>
+      <c r="G1268">
+        <v>0</v>
+      </c>
+      <c r="H1268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:8">
+      <c r="A1269">
+        <v>1268</v>
+      </c>
+      <c r="B1269">
+        <v>3</v>
+      </c>
+      <c r="C1269">
+        <v>4</v>
+      </c>
+      <c r="D1269" t="s">
+        <v>2952</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>2950</v>
+      </c>
+      <c r="F1269" t="s">
+        <v>2953</v>
+      </c>
+      <c r="G1269">
+        <v>0</v>
+      </c>
+      <c r="H1269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:8">
+      <c r="A1270">
+        <v>1269</v>
+      </c>
+      <c r="B1270">
+        <v>3</v>
+      </c>
+      <c r="C1270">
+        <v>4</v>
+      </c>
+      <c r="D1270" t="s">
+        <v>2954</v>
+      </c>
+      <c r="E1270" t="s">
+        <v>2955</v>
+      </c>
+      <c r="F1270" t="s">
+        <v>2953</v>
+      </c>
+      <c r="G1270">
+        <v>0</v>
+      </c>
+      <c r="H1270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:8">
+      <c r="A1271">
+        <v>1270</v>
+      </c>
+      <c r="B1271">
+        <v>3</v>
+      </c>
+      <c r="C1271">
+        <v>4</v>
+      </c>
+      <c r="D1271" t="s">
+        <v>2956</v>
+      </c>
+      <c r="E1271" t="s">
+        <v>2957</v>
+      </c>
+      <c r="F1271" t="s">
+        <v>2958</v>
+      </c>
+      <c r="G1271">
+        <v>0</v>
+      </c>
+      <c r="H1271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:8">
+      <c r="A1272">
+        <v>1271</v>
+      </c>
+      <c r="B1272">
+        <v>3</v>
+      </c>
+      <c r="C1272">
+        <v>4</v>
+      </c>
+      <c r="D1272" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E1272" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F1272" t="s">
+        <v>2958</v>
+      </c>
+      <c r="G1272">
+        <v>0</v>
+      </c>
+      <c r="H1272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:8">
+      <c r="A1273">
+        <v>1272</v>
+      </c>
+      <c r="B1273">
+        <v>3</v>
+      </c>
+      <c r="C1273">
+        <v>4</v>
+      </c>
+      <c r="D1273" t="s">
+        <v>2960</v>
+      </c>
+      <c r="E1273" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F1273" t="s">
+        <v>2961</v>
+      </c>
+      <c r="G1273">
+        <v>0</v>
+      </c>
+      <c r="H1273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:8">
+      <c r="A1274">
+        <v>1273</v>
+      </c>
+      <c r="B1274">
+        <v>3</v>
+      </c>
+      <c r="C1274">
+        <v>4</v>
+      </c>
+      <c r="D1274" t="s">
+        <v>2962</v>
+      </c>
+      <c r="E1274" t="s">
+        <v>2957</v>
+      </c>
+      <c r="F1274" t="s">
+        <v>2963</v>
+      </c>
+      <c r="G1274">
+        <v>0</v>
+      </c>
+      <c r="H1274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:8">
+      <c r="A1275">
+        <v>1274</v>
+      </c>
+      <c r="B1275">
+        <v>3</v>
+      </c>
+      <c r="C1275">
+        <v>4</v>
+      </c>
+      <c r="D1275" t="s">
+        <v>2964</v>
+      </c>
+      <c r="E1275" t="s">
+        <v>2965</v>
+      </c>
+      <c r="F1275" t="s">
+        <v>2966</v>
+      </c>
+      <c r="G1275">
+        <v>0</v>
+      </c>
+      <c r="H1275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:8">
+      <c r="A1276">
+        <v>1275</v>
+      </c>
+      <c r="B1276">
+        <v>3</v>
+      </c>
+      <c r="C1276">
+        <v>4</v>
+      </c>
+      <c r="D1276" t="s">
+        <v>2967</v>
+      </c>
+      <c r="E1276" t="s">
+        <v>2968</v>
+      </c>
+      <c r="F1276" t="s">
+        <v>2966</v>
+      </c>
+      <c r="G1276">
+        <v>0</v>
+      </c>
+      <c r="H1276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:8">
+      <c r="A1277">
+        <v>1276</v>
+      </c>
+      <c r="B1277">
+        <v>3</v>
+      </c>
+      <c r="C1277">
+        <v>4</v>
+      </c>
+      <c r="D1277" t="s">
+        <v>2969</v>
+      </c>
+      <c r="E1277" t="s">
+        <v>2970</v>
+      </c>
+      <c r="F1277" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1277">
+        <v>0</v>
+      </c>
+      <c r="H1277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:8">
+      <c r="A1278">
+        <v>1277</v>
+      </c>
+      <c r="B1278">
+        <v>3</v>
+      </c>
+      <c r="C1278">
+        <v>4</v>
+      </c>
+      <c r="D1278" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E1278" t="s">
+        <v>2970</v>
+      </c>
+      <c r="F1278" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1278">
+        <v>0</v>
+      </c>
+      <c r="H1278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:8">
+      <c r="A1279">
+        <v>1278</v>
+      </c>
+      <c r="B1279">
+        <v>3</v>
+      </c>
+      <c r="C1279">
+        <v>4</v>
+      </c>
+      <c r="D1279" t="s">
+        <v>2973</v>
+      </c>
+      <c r="E1279" t="s">
+        <v>2974</v>
+      </c>
+      <c r="F1279" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1279">
+        <v>0</v>
+      </c>
+      <c r="H1279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:8">
+      <c r="A1280">
+        <v>1279</v>
+      </c>
+      <c r="B1280">
+        <v>3</v>
+      </c>
+      <c r="C1280">
+        <v>4</v>
+      </c>
+      <c r="D1280" t="s">
+        <v>2975</v>
+      </c>
+      <c r="E1280" t="s">
+        <v>2974</v>
+      </c>
+      <c r="F1280" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1280">
+        <v>0</v>
+      </c>
+      <c r="H1280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:8">
+      <c r="A1281">
+        <v>1280</v>
+      </c>
+      <c r="B1281">
+        <v>3</v>
+      </c>
+      <c r="C1281">
+        <v>4</v>
+      </c>
+      <c r="D1281" t="s">
+        <v>2976</v>
+      </c>
+      <c r="E1281" t="s">
+        <v>2977</v>
+      </c>
+      <c r="F1281" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1281">
+        <v>0</v>
+      </c>
+      <c r="H1281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:8">
+      <c r="A1282">
+        <v>1281</v>
+      </c>
+      <c r="B1282">
+        <v>3</v>
+      </c>
+      <c r="C1282">
+        <v>4</v>
+      </c>
+      <c r="D1282" t="s">
+        <v>759</v>
+      </c>
+      <c r="E1282" t="s">
+        <v>2978</v>
+      </c>
+      <c r="F1282" t="s">
+        <v>2979</v>
+      </c>
+      <c r="G1282">
+        <v>0</v>
+      </c>
+      <c r="H1282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:8">
+      <c r="A1283">
+        <v>1282</v>
+      </c>
+      <c r="B1283">
+        <v>3</v>
+      </c>
+      <c r="C1283">
+        <v>4</v>
+      </c>
+      <c r="D1283" t="s">
+        <v>2980</v>
+      </c>
+      <c r="E1283" t="s">
+        <v>2978</v>
+      </c>
+      <c r="F1283" t="s">
+        <v>2981</v>
+      </c>
+      <c r="G1283">
+        <v>0</v>
+      </c>
+      <c r="H1283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:8">
+      <c r="A1284">
+        <v>1283</v>
+      </c>
+      <c r="B1284">
+        <v>3</v>
+      </c>
+      <c r="C1284">
+        <v>4</v>
+      </c>
+      <c r="D1284" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E1284" t="s">
+        <v>2979</v>
+      </c>
+      <c r="F1284" t="s">
+        <v>2981</v>
+      </c>
+      <c r="G1284">
+        <v>0</v>
+      </c>
+      <c r="H1284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:8">
+      <c r="A1285">
+        <v>1284</v>
+      </c>
+      <c r="B1285">
+        <v>3</v>
+      </c>
+      <c r="C1285">
+        <v>4</v>
+      </c>
+      <c r="D1285" t="s">
+        <v>2982</v>
+      </c>
+      <c r="E1285" t="s">
+        <v>2978</v>
+      </c>
+      <c r="F1285" s="2" t="s">
+        <v>2981</v>
+      </c>
+      <c r="G1285">
+        <v>0</v>
+      </c>
+      <c r="H1285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:8">
+      <c r="A1286">
+        <v>1285</v>
+      </c>
+      <c r="B1286">
+        <v>3</v>
+      </c>
+      <c r="C1286">
+        <v>4</v>
+      </c>
+      <c r="D1286" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1286" t="s">
+        <v>2983</v>
+      </c>
+      <c r="F1286" t="s">
+        <v>2984</v>
+      </c>
+      <c r="G1286">
+        <v>0</v>
+      </c>
+      <c r="H1286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:8">
+      <c r="A1287">
+        <v>1286</v>
+      </c>
+      <c r="B1287">
+        <v>3</v>
+      </c>
+      <c r="C1287">
+        <v>4</v>
+      </c>
+      <c r="D1287" t="s">
+        <v>2985</v>
+      </c>
+      <c r="E1287" t="s">
+        <v>2983</v>
+      </c>
+      <c r="F1287" t="s">
+        <v>2986</v>
+      </c>
+      <c r="G1287">
+        <v>0</v>
+      </c>
+      <c r="H1287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:8">
+      <c r="A1288">
+        <v>1287</v>
+      </c>
+      <c r="B1288">
+        <v>3</v>
+      </c>
+      <c r="C1288">
+        <v>4</v>
+      </c>
+      <c r="D1288" t="s">
+        <v>2987</v>
+      </c>
+      <c r="E1288" t="s">
+        <v>2988</v>
+      </c>
+      <c r="F1288" t="s">
+        <v>2989</v>
+      </c>
+      <c r="G1288">
+        <v>0</v>
+      </c>
+      <c r="H1288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:8">
+      <c r="A1289">
+        <v>1288</v>
+      </c>
+      <c r="B1289">
+        <v>3</v>
+      </c>
+      <c r="C1289">
+        <v>4</v>
+      </c>
+      <c r="D1289" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E1289" t="s">
+        <v>2988</v>
+      </c>
+      <c r="F1289" t="s">
+        <v>2990</v>
+      </c>
+      <c r="G1289">
+        <v>0</v>
+      </c>
+      <c r="H1289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:8">
+      <c r="A1290">
+        <v>1289</v>
+      </c>
+      <c r="B1290">
+        <v>3</v>
+      </c>
+      <c r="C1290">
+        <v>4</v>
+      </c>
+      <c r="D1290" t="s">
+        <v>2991</v>
+      </c>
+      <c r="E1290" t="s">
+        <v>2992</v>
+      </c>
+      <c r="F1290" t="s">
+        <v>2989</v>
+      </c>
+      <c r="G1290">
+        <v>0</v>
+      </c>
+      <c r="H1290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:8">
+      <c r="A1291">
+        <v>1290</v>
+      </c>
+      <c r="B1291">
+        <v>3</v>
+      </c>
+      <c r="C1291">
+        <v>4</v>
+      </c>
+      <c r="D1291" t="s">
+        <v>2993</v>
+      </c>
+      <c r="E1291" t="s">
+        <v>2994</v>
+      </c>
+      <c r="F1291" t="s">
+        <v>2995</v>
+      </c>
+      <c r="G1291">
+        <v>0</v>
+      </c>
+      <c r="H1291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:8">
+      <c r="A1292">
+        <v>1291</v>
+      </c>
+      <c r="B1292">
+        <v>3</v>
+      </c>
+      <c r="C1292">
+        <v>4</v>
+      </c>
+      <c r="D1292" t="s">
+        <v>2996</v>
+      </c>
+      <c r="E1292" t="s">
+        <v>2992</v>
+      </c>
+      <c r="F1292" t="s">
+        <v>2995</v>
+      </c>
+      <c r="G1292">
+        <v>0</v>
+      </c>
+      <c r="H1292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:8">
+      <c r="A1293">
+        <v>1292</v>
+      </c>
+      <c r="B1293">
+        <v>3</v>
+      </c>
+      <c r="C1293">
+        <v>4</v>
+      </c>
+      <c r="D1293" t="s">
+        <v>2788</v>
+      </c>
+      <c r="E1293" t="s">
+        <v>2997</v>
+      </c>
+      <c r="F1293" t="s">
+        <v>2998</v>
+      </c>
+      <c r="G1293">
+        <v>0</v>
+      </c>
+      <c r="H1293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:8">
+      <c r="A1294">
+        <v>1293</v>
+      </c>
+      <c r="B1294">
+        <v>3</v>
+      </c>
+      <c r="C1294">
+        <v>4</v>
+      </c>
+      <c r="D1294" t="s">
+        <v>2999</v>
+      </c>
+      <c r="E1294" t="s">
+        <v>3000</v>
+      </c>
+      <c r="F1294" t="s">
+        <v>3001</v>
+      </c>
+      <c r="G1294">
+        <v>0</v>
+      </c>
+      <c r="H1294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:8">
+      <c r="A1295">
+        <v>1294</v>
+      </c>
+      <c r="B1295">
+        <v>3</v>
+      </c>
+      <c r="C1295">
+        <v>4</v>
+      </c>
+      <c r="D1295" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1295" t="s">
+        <v>3000</v>
+      </c>
+      <c r="F1295" t="s">
+        <v>3002</v>
+      </c>
+      <c r="G1295">
+        <v>0</v>
+      </c>
+      <c r="H1295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:8">
+      <c r="A1296">
+        <v>1295</v>
+      </c>
+      <c r="B1296">
+        <v>3</v>
+      </c>
+      <c r="C1296">
+        <v>4</v>
+      </c>
+      <c r="D1296" t="s">
+        <v>2074</v>
+      </c>
+      <c r="E1296" t="s">
+        <v>3003</v>
+      </c>
+      <c r="F1296" t="s">
+        <v>3001</v>
+      </c>
+      <c r="G1296">
+        <v>0</v>
+      </c>
+      <c r="H1296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:8">
+      <c r="A1297">
+        <v>1296</v>
+      </c>
+      <c r="B1297">
+        <v>3</v>
+      </c>
+      <c r="C1297">
+        <v>4</v>
+      </c>
+      <c r="D1297" t="s">
+        <v>3004</v>
+      </c>
+      <c r="E1297" t="s">
+        <v>3003</v>
+      </c>
+      <c r="F1297" t="s">
+        <v>3005</v>
+      </c>
+      <c r="G1297">
+        <v>0</v>
+      </c>
+      <c r="H1297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:8">
+      <c r="A1298">
+        <v>1297</v>
+      </c>
+      <c r="B1298">
+        <v>3</v>
+      </c>
+      <c r="C1298">
+        <v>4</v>
+      </c>
+      <c r="D1298" t="s">
+        <v>3006</v>
+      </c>
+      <c r="E1298" t="s">
+        <v>3007</v>
+      </c>
+      <c r="F1298" t="s">
+        <v>3005</v>
+      </c>
+      <c r="G1298">
+        <v>0</v>
+      </c>
+      <c r="H1298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:8">
+      <c r="A1299">
+        <v>1298</v>
+      </c>
+      <c r="B1299">
+        <v>3</v>
+      </c>
+      <c r="C1299">
+        <v>4</v>
+      </c>
+      <c r="D1299" t="s">
+        <v>3008</v>
+      </c>
+      <c r="E1299" t="s">
+        <v>3007</v>
+      </c>
+      <c r="F1299" t="s">
+        <v>3009</v>
+      </c>
+      <c r="G1299">
+        <v>0</v>
+      </c>
+      <c r="H1299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:8">
+      <c r="A1300">
+        <v>1299</v>
+      </c>
+      <c r="B1300">
+        <v>3</v>
+      </c>
+      <c r="C1300">
+        <v>4</v>
+      </c>
+      <c r="D1300" t="s">
+        <v>2406</v>
+      </c>
+      <c r="E1300" t="s">
+        <v>3010</v>
+      </c>
+      <c r="F1300" t="s">
+        <v>3011</v>
+      </c>
+      <c r="G1300">
+        <v>0</v>
+      </c>
+      <c r="H1300">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove 100+ words because they were logged with non-drop timeframes
</commit_message>
<xml_diff>
--- a/spreadsheets/clips.xlsx
+++ b/spreadsheets/clips.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7424" uniqueCount="5665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7112" uniqueCount="5428">
   <si>
     <t>id</t>
   </si>
@@ -16306,717 +16306,6 @@
   </si>
   <si>
     <t>00;08;20;54</t>
-  </si>
-  <si>
-    <t>a very</t>
-  </si>
-  <si>
-    <t>00:08:20:21</t>
-  </si>
-  <si>
-    <t>00:08:21:04</t>
-  </si>
-  <si>
-    <t>00:08:20:35</t>
-  </si>
-  <si>
-    <t>00:08:21:05</t>
-  </si>
-  <si>
-    <t>00:08:21:40</t>
-  </si>
-  <si>
-    <t>00:08:21:41</t>
-  </si>
-  <si>
-    <t>00:08:22:12</t>
-  </si>
-  <si>
-    <t>thats it</t>
-  </si>
-  <si>
-    <t>00:08:24:57</t>
-  </si>
-  <si>
-    <t>00:08:25:25</t>
-  </si>
-  <si>
-    <t>that's it</t>
-  </si>
-  <si>
-    <t>fox 32 news</t>
-  </si>
-  <si>
-    <t>00:08:25:32</t>
-  </si>
-  <si>
-    <t>00:08:26:34</t>
-  </si>
-  <si>
-    <t>00:08:25:50</t>
-  </si>
-  <si>
-    <t>thirty two</t>
-  </si>
-  <si>
-    <t>00:08:26:18</t>
-  </si>
-  <si>
-    <t>news</t>
-  </si>
-  <si>
-    <t>00:08:26:15</t>
-  </si>
-  <si>
-    <t>00:08:26:35</t>
-  </si>
-  <si>
-    <t>00:08:26:49</t>
-  </si>
-  <si>
-    <t>thank you</t>
-  </si>
-  <si>
-    <t>00:08:27:07</t>
-  </si>
-  <si>
-    <t>so much</t>
-  </si>
-  <si>
-    <t>00:08:27:08</t>
-  </si>
-  <si>
-    <t>00:08:27:47</t>
-  </si>
-  <si>
-    <t>so much for</t>
-  </si>
-  <si>
-    <t>00:08:27:55</t>
-  </si>
-  <si>
-    <t>joining us</t>
-  </si>
-  <si>
-    <t>00:08:27:53</t>
-  </si>
-  <si>
-    <t>00:08:28:27</t>
-  </si>
-  <si>
-    <t>00:08:28:28</t>
-  </si>
-  <si>
-    <t>00:08:28:47</t>
-  </si>
-  <si>
-    <t>00:08:29:08</t>
-  </si>
-  <si>
-    <t>00:08:29:29</t>
-  </si>
-  <si>
-    <t>returns</t>
-  </si>
-  <si>
-    <t>00:08:29:30</t>
-  </si>
-  <si>
-    <t>00:08:30:03</t>
-  </si>
-  <si>
-    <t>tomorrow morning</t>
-  </si>
-  <si>
-    <t>00:08:30:01</t>
-  </si>
-  <si>
-    <t>00:08:30:46</t>
-  </si>
-  <si>
-    <t>four thirty</t>
-  </si>
-  <si>
-    <t>00:08:31:00</t>
-  </si>
-  <si>
-    <t>00:08:31:49</t>
-  </si>
-  <si>
-    <t>00:08:31:14</t>
-  </si>
-  <si>
-    <t>00:08:30:53</t>
-  </si>
-  <si>
-    <t>00:08:31:16</t>
-  </si>
-  <si>
-    <t>a.m.</t>
-  </si>
-  <si>
-    <t>00:08:31:47</t>
-  </si>
-  <si>
-    <t>00:08:32:37</t>
-  </si>
-  <si>
-    <t>starts</t>
-  </si>
-  <si>
-    <t>00:08:33:31</t>
-  </si>
-  <si>
-    <t>00:08:33:58</t>
-  </si>
-  <si>
-    <t>final words</t>
-  </si>
-  <si>
-    <t>00:08:32:43</t>
-  </si>
-  <si>
-    <t>00:08:33:35</t>
-  </si>
-  <si>
-    <t>final word</t>
-  </si>
-  <si>
-    <t>00:08:32:42</t>
-  </si>
-  <si>
-    <t>00:08:33:06</t>
-  </si>
-  <si>
-    <t>00:08:33:07</t>
-  </si>
-  <si>
-    <t>00:08:33:34</t>
-  </si>
-  <si>
-    <t>right after</t>
-  </si>
-  <si>
-    <t>00:08:33:59</t>
-  </si>
-  <si>
-    <t>00:08:34:26</t>
-  </si>
-  <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>00:11:40:20</t>
-  </si>
-  <si>
-    <t>00:11:40:55</t>
-  </si>
-  <si>
-    <t>reboot</t>
-  </si>
-  <si>
-    <t>00:11:41:36</t>
-  </si>
-  <si>
-    <t>00:11:42:05</t>
-  </si>
-  <si>
-    <t>can't wait</t>
-  </si>
-  <si>
-    <t>00:11:43:34</t>
-  </si>
-  <si>
-    <t>00:11:44:05</t>
-  </si>
-  <si>
-    <t>can't wait to</t>
-  </si>
-  <si>
-    <t>00:11:44:14</t>
-  </si>
-  <si>
-    <t>wait to</t>
-  </si>
-  <si>
-    <t>00:11:43:46</t>
-  </si>
-  <si>
-    <t>wait</t>
-  </si>
-  <si>
-    <t>00:11:44:03</t>
-  </si>
-  <si>
-    <t>and soon</t>
-  </si>
-  <si>
-    <t>00:11:45:30</t>
-  </si>
-  <si>
-    <t>00:11:46:02</t>
-  </si>
-  <si>
-    <t>00:11:45:42</t>
-  </si>
-  <si>
-    <t>we will</t>
-  </si>
-  <si>
-    <t>00:11:46:24</t>
-  </si>
-  <si>
-    <t>kick off</t>
-  </si>
-  <si>
-    <t>00:11:46:25</t>
-  </si>
-  <si>
-    <t>00:11:46:47</t>
-  </si>
-  <si>
-    <t>kickoff</t>
-  </si>
-  <si>
-    <t>00:11:46:20</t>
-  </si>
-  <si>
-    <t>00:11:46:36</t>
-  </si>
-  <si>
-    <t>00:11:47:08</t>
-  </si>
-  <si>
-    <t>all those</t>
-  </si>
-  <si>
-    <t>00:11:49:25</t>
-  </si>
-  <si>
-    <t>00:11:49:55</t>
-  </si>
-  <si>
-    <t>00:11:49:23</t>
-  </si>
-  <si>
-    <t>00:11:49:40</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>00:11:49:47</t>
-  </si>
-  <si>
-    <t>00:11:50:24</t>
-  </si>
-  <si>
-    <t>topics</t>
-  </si>
-  <si>
-    <t>00:11:50:29</t>
-  </si>
-  <si>
-    <t>and more</t>
-  </si>
-  <si>
-    <t>00:11:50:30</t>
-  </si>
-  <si>
-    <t>00:11:51:23</t>
-  </si>
-  <si>
-    <t>00:11:51:03</t>
-  </si>
-  <si>
-    <t>00:11:51:02</t>
-  </si>
-  <si>
-    <t>00:11:51:24</t>
-  </si>
-  <si>
-    <t>00:11:51:25</t>
-  </si>
-  <si>
-    <t>00:11:51:47</t>
-  </si>
-  <si>
-    <t>here on the</t>
-  </si>
-  <si>
-    <t>00:11:51:45</t>
-  </si>
-  <si>
-    <t>00:11:52:09</t>
-  </si>
-  <si>
-    <t>here on</t>
-  </si>
-  <si>
-    <t>00:11:52:03</t>
-  </si>
-  <si>
-    <t>heron</t>
-  </si>
-  <si>
-    <t>00:11:52:12</t>
-  </si>
-  <si>
-    <t>00:11:52:51</t>
-  </si>
-  <si>
-    <t>00:11:52:30</t>
-  </si>
-  <si>
-    <t>under the weather</t>
-  </si>
-  <si>
-    <t>00:11:56:24</t>
-  </si>
-  <si>
-    <t>00:11:57:14</t>
-  </si>
-  <si>
-    <t>chicago tribune</t>
-  </si>
-  <si>
-    <t>00:11:57:27</t>
-  </si>
-  <si>
-    <t>00:11:58:21</t>
-  </si>
-  <si>
-    <t>teddy</t>
-  </si>
-  <si>
-    <t>00:11:58:22</t>
-  </si>
-  <si>
-    <t>00:11:58:37</t>
-  </si>
-  <si>
-    <t>00:11:59:11</t>
-  </si>
-  <si>
-    <t>00:11:59:31</t>
-  </si>
-  <si>
-    <t>see ya</t>
-  </si>
-  <si>
-    <t>00:11:59:42</t>
-  </si>
-  <si>
-    <t>00:12:00:08</t>
-  </si>
-  <si>
-    <t>00:12:00:27</t>
-  </si>
-  <si>
-    <t>00:12:00:46</t>
-  </si>
-  <si>
-    <t>be here</t>
-  </si>
-  <si>
-    <t>00:12:00:45</t>
-  </si>
-  <si>
-    <t>00:12:01:03</t>
-  </si>
-  <si>
-    <t>00:12:01:00</t>
-  </si>
-  <si>
-    <t>00:12:01:40</t>
-  </si>
-  <si>
-    <t>great to have</t>
-  </si>
-  <si>
-    <t>00:12:01:41</t>
-  </si>
-  <si>
-    <t>00:12:02:15</t>
-  </si>
-  <si>
-    <t>to have</t>
-  </si>
-  <si>
-    <t>00:12:01:51</t>
-  </si>
-  <si>
-    <t>00:12:05:25</t>
-  </si>
-  <si>
-    <t>00:12:05:48</t>
-  </si>
-  <si>
-    <t>00:12:05:49</t>
-  </si>
-  <si>
-    <t>00:12:07:01</t>
-  </si>
-  <si>
-    <t>as embarrassing</t>
-  </si>
-  <si>
-    <t>embarrassing</t>
-  </si>
-  <si>
-    <t>00:12:06:09</t>
-  </si>
-  <si>
-    <t>i've seen</t>
-  </si>
-  <si>
-    <t>00:12:07:44</t>
-  </si>
-  <si>
-    <t>00:12:08:10</t>
-  </si>
-  <si>
-    <t>00:12:07:48</t>
-  </si>
-  <si>
-    <t>franchise</t>
-  </si>
-  <si>
-    <t>00:12:08:30</t>
-  </si>
-  <si>
-    <t>00:12:09:10</t>
-  </si>
-  <si>
-    <t>in a long</t>
-  </si>
-  <si>
-    <t>00:12:09:11</t>
-  </si>
-  <si>
-    <t>00:12:10:12</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>00:12:09:39</t>
-  </si>
-  <si>
-    <t>00:12:10:13</t>
-  </si>
-  <si>
-    <t>long time</t>
-  </si>
-  <si>
-    <t>00:12:10:49</t>
-  </si>
-  <si>
-    <t>00:12:10:50</t>
-  </si>
-  <si>
-    <t>00:12:11:03</t>
-  </si>
-  <si>
-    <t>mark</t>
-  </si>
-  <si>
-    <t>00:12:11:16</t>
-  </si>
-  <si>
-    <t>00:12:11:33</t>
-  </si>
-  <si>
-    <t>needs to</t>
-  </si>
-  <si>
-    <t>00:12:11:51</t>
-  </si>
-  <si>
-    <t>00:12:12:15</t>
-  </si>
-  <si>
-    <t>00:12:12:16</t>
-  </si>
-  <si>
-    <t>00:12:12:47</t>
-  </si>
-  <si>
-    <t>maybe</t>
-  </si>
-  <si>
-    <t>00:12:13:51</t>
-  </si>
-  <si>
-    <t>00:12:14:09</t>
-  </si>
-  <si>
-    <t>book a trip</t>
-  </si>
-  <si>
-    <t>00:12:14:10</t>
-  </si>
-  <si>
-    <t>00:12:14:38</t>
-  </si>
-  <si>
-    <t>trip to</t>
-  </si>
-  <si>
-    <t>00:12:14:24</t>
-  </si>
-  <si>
-    <t>00:12:14:45</t>
-  </si>
-  <si>
-    <t>trip</t>
-  </si>
-  <si>
-    <t>00:12:14:22</t>
-  </si>
-  <si>
-    <t>00:12:14:37</t>
-  </si>
-  <si>
-    <t>to hawaii</t>
-  </si>
-  <si>
-    <t>00:12:15:16</t>
-  </si>
-  <si>
-    <t>hawaii</t>
-  </si>
-  <si>
-    <t>00:12:15:22</t>
-  </si>
-  <si>
-    <t>00:12:15:53</t>
-  </si>
-  <si>
-    <t>i don't</t>
-  </si>
-  <si>
-    <t>00:12:15:45</t>
-  </si>
-  <si>
-    <t>00:12:15:40</t>
-  </si>
-  <si>
-    <t>00:12:15:56</t>
-  </si>
-  <si>
-    <t>this man</t>
-  </si>
-  <si>
-    <t>00:12:15:51</t>
-  </si>
-  <si>
-    <t>00:12:16:17</t>
-  </si>
-  <si>
-    <t>00:12:16:05</t>
-  </si>
-  <si>
-    <t>come home</t>
-  </si>
-  <si>
-    <t>00:12:16:33</t>
-  </si>
-  <si>
-    <t>00:12:16:51</t>
-  </si>
-  <si>
-    <t>00:12:16:32</t>
-  </si>
-  <si>
-    <t>00:12:16:44</t>
-  </si>
-  <si>
-    <t>00:12:16:52</t>
-  </si>
-  <si>
-    <t>00:12:17:13</t>
-  </si>
-  <si>
-    <t>touch</t>
-  </si>
-  <si>
-    <t>00:12:19:31</t>
-  </si>
-  <si>
-    <t>00:12:19:47</t>
-  </si>
-  <si>
-    <t>touch on</t>
-  </si>
-  <si>
-    <t>00:12:19:56</t>
-  </si>
-  <si>
-    <t>we will talk</t>
-  </si>
-  <si>
-    <t>00:12:20:39</t>
-  </si>
-  <si>
-    <t>00:12:21:02</t>
-  </si>
-  <si>
-    <t>00:12:20:47</t>
-  </si>
-  <si>
-    <t>plenty</t>
-  </si>
-  <si>
-    <t>00:12:21:00</t>
-  </si>
-  <si>
-    <t>00:12:21:19</t>
-  </si>
-  <si>
-    <t>beat</t>
-  </si>
-  <si>
-    <t>00:12:23:30</t>
-  </si>
-  <si>
-    <t>00:12:23:55</t>
-  </si>
-  <si>
-    <t>00:12:25:06</t>
-  </si>
-  <si>
-    <t>00:12:25:28</t>
-  </si>
-  <si>
-    <t>last night</t>
-  </si>
-  <si>
-    <t>00:12:25:29</t>
-  </si>
-  <si>
-    <t>00:12:25:53</t>
-  </si>
-  <si>
-    <t>last nights</t>
-  </si>
-  <si>
-    <t>00:12:25:56</t>
-  </si>
-  <si>
-    <t>spartans</t>
-  </si>
-  <si>
-    <t>00:12:27:56</t>
-  </si>
-  <si>
-    <t>00:12:28:22</t>
-  </si>
-  <si>
-    <t>thirteen</t>
-  </si>
-  <si>
-    <t>00:12:28:43</t>
   </si>
 </sst>
 </file>
@@ -17076,8 +16365,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="453">
+  <cellStyleXfs count="497">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -17536,7 +16869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="453">
+  <cellStyles count="497">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -17763,6 +17096,28 @@
     <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -17989,6 +17344,28 @@
     <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -18318,10 +17695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2500"/>
+  <dimension ref="A1:H2369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2462" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F2473" sqref="F2473"/>
+    <sheetView tabSelected="1" topLeftCell="A2358" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C2374" sqref="C2374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -79928,3169 +79305,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2370" spans="1:8">
-      <c r="A2370">
-        <v>2369</v>
-      </c>
-      <c r="B2370">
-        <v>1</v>
-      </c>
-      <c r="C2370">
-        <v>7</v>
-      </c>
-      <c r="D2370" t="s">
-        <v>5428</v>
-      </c>
-      <c r="E2370" t="s">
-        <v>5429</v>
-      </c>
-      <c r="F2370" t="s">
-        <v>5430</v>
-      </c>
-      <c r="G2370">
-        <v>0</v>
-      </c>
-      <c r="H2370">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2371" spans="1:8">
-      <c r="A2371">
-        <v>2370</v>
-      </c>
-      <c r="B2371">
-        <v>1</v>
-      </c>
-      <c r="C2371">
-        <v>7</v>
-      </c>
-      <c r="D2371" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2371" t="s">
-        <v>5431</v>
-      </c>
-      <c r="F2371" t="s">
-        <v>5430</v>
-      </c>
-      <c r="G2371">
-        <v>0</v>
-      </c>
-      <c r="H2371">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2372" spans="1:8">
-      <c r="A2372">
-        <v>2371</v>
-      </c>
-      <c r="B2372">
-        <v>1</v>
-      </c>
-      <c r="C2372">
-        <v>7</v>
-      </c>
-      <c r="D2372" t="s">
-        <v>722</v>
-      </c>
-      <c r="E2372" t="s">
-        <v>5432</v>
-      </c>
-      <c r="F2372" t="s">
-        <v>5433</v>
-      </c>
-      <c r="G2372">
-        <v>0</v>
-      </c>
-      <c r="H2372">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2373" spans="1:8">
-      <c r="A2373">
-        <v>2372</v>
-      </c>
-      <c r="B2373">
-        <v>1</v>
-      </c>
-      <c r="C2373">
-        <v>7</v>
-      </c>
-      <c r="D2373" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E2373" t="s">
-        <v>5434</v>
-      </c>
-      <c r="F2373" t="s">
-        <v>5435</v>
-      </c>
-      <c r="G2373">
-        <v>0</v>
-      </c>
-      <c r="H2373">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2374" spans="1:8">
-      <c r="A2374">
-        <v>2373</v>
-      </c>
-      <c r="B2374">
-        <v>1</v>
-      </c>
-      <c r="C2374">
-        <v>7</v>
-      </c>
-      <c r="D2374" t="s">
-        <v>5436</v>
-      </c>
-      <c r="E2374" t="s">
-        <v>5437</v>
-      </c>
-      <c r="F2374" t="s">
-        <v>5438</v>
-      </c>
-      <c r="G2374">
-        <v>0</v>
-      </c>
-      <c r="H2374">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2375" spans="1:8">
-      <c r="A2375">
-        <v>2374</v>
-      </c>
-      <c r="B2375">
-        <v>1</v>
-      </c>
-      <c r="C2375">
-        <v>7</v>
-      </c>
-      <c r="D2375" t="s">
-        <v>5439</v>
-      </c>
-      <c r="E2375" t="s">
-        <v>5437</v>
-      </c>
-      <c r="F2375" t="s">
-        <v>5438</v>
-      </c>
-      <c r="G2375">
-        <v>0</v>
-      </c>
-      <c r="H2375">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2376" spans="1:8">
-      <c r="A2376">
-        <v>2375</v>
-      </c>
-      <c r="B2376">
-        <v>1</v>
-      </c>
-      <c r="C2376">
-        <v>7</v>
-      </c>
-      <c r="D2376" t="s">
-        <v>5440</v>
-      </c>
-      <c r="E2376" t="s">
-        <v>5441</v>
-      </c>
-      <c r="F2376" t="s">
-        <v>5442</v>
-      </c>
-      <c r="G2376">
-        <v>0</v>
-      </c>
-      <c r="H2376">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2377" spans="1:8">
-      <c r="A2377">
-        <v>2376</v>
-      </c>
-      <c r="B2377">
-        <v>1</v>
-      </c>
-      <c r="C2377">
-        <v>7</v>
-      </c>
-      <c r="D2377" t="s">
-        <v>862</v>
-      </c>
-      <c r="E2377" t="s">
-        <v>5441</v>
-      </c>
-      <c r="F2377" t="s">
-        <v>5443</v>
-      </c>
-      <c r="G2377">
-        <v>0</v>
-      </c>
-      <c r="H2377">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2378" spans="1:8">
-      <c r="A2378">
-        <v>2377</v>
-      </c>
-      <c r="B2378">
-        <v>1</v>
-      </c>
-      <c r="C2378">
-        <v>7</v>
-      </c>
-      <c r="D2378" t="s">
-        <v>5444</v>
-      </c>
-      <c r="E2378" t="s">
-        <v>5443</v>
-      </c>
-      <c r="F2378" t="s">
-        <v>5445</v>
-      </c>
-      <c r="G2378">
-        <v>0</v>
-      </c>
-      <c r="H2378">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2379" spans="1:8">
-      <c r="A2379">
-        <v>2378</v>
-      </c>
-      <c r="B2379">
-        <v>1</v>
-      </c>
-      <c r="C2379">
-        <v>7</v>
-      </c>
-      <c r="D2379" t="s">
-        <v>5446</v>
-      </c>
-      <c r="E2379" t="s">
-        <v>5447</v>
-      </c>
-      <c r="F2379" t="s">
-        <v>5448</v>
-      </c>
-      <c r="G2379">
-        <v>0</v>
-      </c>
-      <c r="H2379">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2380" spans="1:8">
-      <c r="A2380">
-        <v>2379</v>
-      </c>
-      <c r="B2380">
-        <v>1</v>
-      </c>
-      <c r="C2380">
-        <v>7</v>
-      </c>
-      <c r="D2380" t="s">
-        <v>5450</v>
-      </c>
-      <c r="E2380" t="s">
-        <v>5449</v>
-      </c>
-      <c r="F2380" t="s">
-        <v>5451</v>
-      </c>
-      <c r="G2380">
-        <v>0</v>
-      </c>
-      <c r="H2380">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2381" spans="1:8">
-      <c r="A2381">
-        <v>2380</v>
-      </c>
-      <c r="B2381">
-        <v>1</v>
-      </c>
-      <c r="C2381">
-        <v>7</v>
-      </c>
-      <c r="D2381" t="s">
-        <v>5452</v>
-      </c>
-      <c r="E2381" t="s">
-        <v>5453</v>
-      </c>
-      <c r="F2381" t="s">
-        <v>5454</v>
-      </c>
-      <c r="G2381">
-        <v>0</v>
-      </c>
-      <c r="H2381">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2382" spans="1:8">
-      <c r="A2382">
-        <v>2381</v>
-      </c>
-      <c r="B2382">
-        <v>1</v>
-      </c>
-      <c r="C2382">
-        <v>7</v>
-      </c>
-      <c r="D2382" t="s">
-        <v>5455</v>
-      </c>
-      <c r="E2382" t="s">
-        <v>5453</v>
-      </c>
-      <c r="F2382" t="s">
-        <v>5456</v>
-      </c>
-      <c r="G2382">
-        <v>0</v>
-      </c>
-      <c r="H2382">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2383" spans="1:8">
-      <c r="A2383">
-        <v>2382</v>
-      </c>
-      <c r="B2383">
-        <v>1</v>
-      </c>
-      <c r="C2383">
-        <v>7</v>
-      </c>
-      <c r="D2383" t="s">
-        <v>5457</v>
-      </c>
-      <c r="E2383" t="s">
-        <v>5458</v>
-      </c>
-      <c r="F2383" t="s">
-        <v>5459</v>
-      </c>
-      <c r="G2383">
-        <v>0</v>
-      </c>
-      <c r="H2383">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2384" spans="1:8">
-      <c r="A2384">
-        <v>2383</v>
-      </c>
-      <c r="B2384">
-        <v>1</v>
-      </c>
-      <c r="C2384">
-        <v>7</v>
-      </c>
-      <c r="D2384" t="s">
-        <v>862</v>
-      </c>
-      <c r="E2384" t="s">
-        <v>5460</v>
-      </c>
-      <c r="F2384" t="s">
-        <v>5461</v>
-      </c>
-      <c r="G2384">
-        <v>0</v>
-      </c>
-      <c r="H2384">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2385" spans="1:8">
-      <c r="A2385">
-        <v>2384</v>
-      </c>
-      <c r="B2385">
-        <v>1</v>
-      </c>
-      <c r="C2385">
-        <v>7</v>
-      </c>
-      <c r="D2385" t="s">
-        <v>5446</v>
-      </c>
-      <c r="E2385" t="s">
-        <v>5462</v>
-      </c>
-      <c r="F2385" t="s">
-        <v>5463</v>
-      </c>
-      <c r="G2385">
-        <v>0</v>
-      </c>
-      <c r="H2385">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2386" spans="1:8">
-      <c r="A2386">
-        <v>2385</v>
-      </c>
-      <c r="B2386">
-        <v>1</v>
-      </c>
-      <c r="C2386">
-        <v>7</v>
-      </c>
-      <c r="D2386" t="s">
-        <v>5464</v>
-      </c>
-      <c r="E2386" t="s">
-        <v>5465</v>
-      </c>
-      <c r="F2386" t="s">
-        <v>5466</v>
-      </c>
-      <c r="G2386">
-        <v>0</v>
-      </c>
-      <c r="H2386">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2387" spans="1:8">
-      <c r="A2387">
-        <v>2386</v>
-      </c>
-      <c r="B2387">
-        <v>1</v>
-      </c>
-      <c r="C2387">
-        <v>7</v>
-      </c>
-      <c r="D2387" t="s">
-        <v>5467</v>
-      </c>
-      <c r="E2387" t="s">
-        <v>5468</v>
-      </c>
-      <c r="F2387" t="s">
-        <v>5469</v>
-      </c>
-      <c r="G2387">
-        <v>0</v>
-      </c>
-      <c r="H2387">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2388" spans="1:8">
-      <c r="A2388">
-        <v>2387</v>
-      </c>
-      <c r="B2388">
-        <v>1</v>
-      </c>
-      <c r="C2388">
-        <v>7</v>
-      </c>
-      <c r="D2388" t="s">
-        <v>5470</v>
-      </c>
-      <c r="E2388" t="s">
-        <v>5471</v>
-      </c>
-      <c r="F2388" t="s">
-        <v>5472</v>
-      </c>
-      <c r="G2388">
-        <v>0</v>
-      </c>
-      <c r="H2388">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2389" spans="1:8">
-      <c r="A2389">
-        <v>2388</v>
-      </c>
-      <c r="B2389">
-        <v>1</v>
-      </c>
-      <c r="C2389">
-        <v>7</v>
-      </c>
-      <c r="D2389" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E2389" t="s">
-        <v>5473</v>
-      </c>
-      <c r="F2389" t="s">
-        <v>5472</v>
-      </c>
-      <c r="G2389">
-        <v>0</v>
-      </c>
-      <c r="H2389">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2390" spans="1:8">
-      <c r="A2390">
-        <v>2389</v>
-      </c>
-      <c r="B2390">
-        <v>1</v>
-      </c>
-      <c r="C2390">
-        <v>7</v>
-      </c>
-      <c r="D2390" t="s">
-        <v>700</v>
-      </c>
-      <c r="E2390" t="s">
-        <v>5474</v>
-      </c>
-      <c r="F2390" t="s">
-        <v>5475</v>
-      </c>
-      <c r="G2390">
-        <v>0</v>
-      </c>
-      <c r="H2390">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2391" spans="1:8">
-      <c r="A2391">
-        <v>2390</v>
-      </c>
-      <c r="B2391">
-        <v>1</v>
-      </c>
-      <c r="C2391">
-        <v>7</v>
-      </c>
-      <c r="D2391" t="s">
-        <v>271</v>
-      </c>
-      <c r="E2391" t="s">
-        <v>5474</v>
-      </c>
-      <c r="F2391" t="s">
-        <v>5475</v>
-      </c>
-      <c r="G2391">
-        <v>0</v>
-      </c>
-      <c r="H2391">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2392" spans="1:8">
-      <c r="A2392">
-        <v>2391</v>
-      </c>
-      <c r="B2392">
-        <v>1</v>
-      </c>
-      <c r="C2392">
-        <v>7</v>
-      </c>
-      <c r="D2392" t="s">
-        <v>5476</v>
-      </c>
-      <c r="E2392" t="s">
-        <v>5477</v>
-      </c>
-      <c r="F2392" t="s">
-        <v>5478</v>
-      </c>
-      <c r="G2392">
-        <v>0</v>
-      </c>
-      <c r="H2392">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2393" spans="1:8">
-      <c r="A2393">
-        <v>2392</v>
-      </c>
-      <c r="B2393">
-        <v>1</v>
-      </c>
-      <c r="C2393">
-        <v>7</v>
-      </c>
-      <c r="D2393" t="s">
-        <v>5479</v>
-      </c>
-      <c r="E2393" t="s">
-        <v>5480</v>
-      </c>
-      <c r="F2393" t="s">
-        <v>5481</v>
-      </c>
-      <c r="G2393">
-        <v>0</v>
-      </c>
-      <c r="H2393">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2394" spans="1:8">
-      <c r="A2394">
-        <v>2393</v>
-      </c>
-      <c r="B2394">
-        <v>1</v>
-      </c>
-      <c r="C2394">
-        <v>7</v>
-      </c>
-      <c r="D2394" t="s">
-        <v>5482</v>
-      </c>
-      <c r="E2394" t="s">
-        <v>5483</v>
-      </c>
-      <c r="F2394" t="s">
-        <v>5484</v>
-      </c>
-      <c r="G2394">
-        <v>0</v>
-      </c>
-      <c r="H2394">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2395" spans="1:8">
-      <c r="A2395">
-        <v>2394</v>
-      </c>
-      <c r="B2395">
-        <v>1</v>
-      </c>
-      <c r="C2395">
-        <v>7</v>
-      </c>
-      <c r="D2395" t="s">
-        <v>5485</v>
-      </c>
-      <c r="E2395" t="s">
-        <v>5483</v>
-      </c>
-      <c r="F2395" t="s">
-        <v>5480</v>
-      </c>
-      <c r="G2395">
-        <v>0</v>
-      </c>
-      <c r="H2395">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2396" spans="1:8">
-      <c r="A2396">
-        <v>2395</v>
-      </c>
-      <c r="B2396">
-        <v>1</v>
-      </c>
-      <c r="C2396">
-        <v>7</v>
-      </c>
-      <c r="D2396" t="s">
-        <v>4966</v>
-      </c>
-      <c r="E2396" t="s">
-        <v>5486</v>
-      </c>
-      <c r="F2396" t="s">
-        <v>5487</v>
-      </c>
-      <c r="G2396">
-        <v>0</v>
-      </c>
-      <c r="H2396">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2397" spans="1:8">
-      <c r="A2397">
-        <v>2396</v>
-      </c>
-      <c r="B2397">
-        <v>1</v>
-      </c>
-      <c r="C2397">
-        <v>7</v>
-      </c>
-      <c r="D2397" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2397" t="s">
-        <v>5488</v>
-      </c>
-      <c r="F2397" t="s">
-        <v>5489</v>
-      </c>
-      <c r="G2397">
-        <v>0</v>
-      </c>
-      <c r="H2397">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2398" spans="1:8">
-      <c r="A2398">
-        <v>2397</v>
-      </c>
-      <c r="B2398">
-        <v>1</v>
-      </c>
-      <c r="C2398">
-        <v>7</v>
-      </c>
-      <c r="D2398" t="s">
-        <v>5490</v>
-      </c>
-      <c r="E2398" t="s">
-        <v>5491</v>
-      </c>
-      <c r="F2398" t="s">
-        <v>5492</v>
-      </c>
-      <c r="G2398">
-        <v>0</v>
-      </c>
-      <c r="H2398">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2399" spans="1:8">
-      <c r="A2399">
-        <v>2398</v>
-      </c>
-      <c r="B2399">
-        <v>1</v>
-      </c>
-      <c r="C2399">
-        <v>7</v>
-      </c>
-      <c r="D2399" t="s">
-        <v>5493</v>
-      </c>
-      <c r="E2399" t="s">
-        <v>5494</v>
-      </c>
-      <c r="F2399" t="s">
-        <v>5495</v>
-      </c>
-      <c r="G2399">
-        <v>0</v>
-      </c>
-      <c r="H2399">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2400" spans="1:8">
-      <c r="A2400">
-        <v>2399</v>
-      </c>
-      <c r="B2400">
-        <v>1</v>
-      </c>
-      <c r="C2400">
-        <v>7</v>
-      </c>
-      <c r="D2400" t="s">
-        <v>5496</v>
-      </c>
-      <c r="E2400" t="s">
-        <v>5497</v>
-      </c>
-      <c r="F2400" t="s">
-        <v>5498</v>
-      </c>
-      <c r="G2400">
-        <v>0</v>
-      </c>
-      <c r="H2400">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2401" spans="1:8">
-      <c r="A2401">
-        <v>2400</v>
-      </c>
-      <c r="B2401">
-        <v>1</v>
-      </c>
-      <c r="C2401">
-        <v>7</v>
-      </c>
-      <c r="D2401" t="s">
-        <v>5499</v>
-      </c>
-      <c r="E2401" t="s">
-        <v>5500</v>
-      </c>
-      <c r="F2401" t="s">
-        <v>5501</v>
-      </c>
-      <c r="G2401">
-        <v>0</v>
-      </c>
-      <c r="H2401">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2402" spans="1:8">
-      <c r="A2402">
-        <v>2401</v>
-      </c>
-      <c r="B2402">
-        <v>1</v>
-      </c>
-      <c r="C2402">
-        <v>7</v>
-      </c>
-      <c r="D2402" t="s">
-        <v>5502</v>
-      </c>
-      <c r="E2402" t="s">
-        <v>5500</v>
-      </c>
-      <c r="F2402" t="s">
-        <v>5503</v>
-      </c>
-      <c r="G2402">
-        <v>0</v>
-      </c>
-      <c r="H2402">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2403" spans="1:8">
-      <c r="A2403">
-        <v>2402</v>
-      </c>
-      <c r="B2403">
-        <v>1</v>
-      </c>
-      <c r="C2403">
-        <v>7</v>
-      </c>
-      <c r="D2403" t="s">
-        <v>5504</v>
-      </c>
-      <c r="E2403" t="s">
-        <v>5505</v>
-      </c>
-      <c r="F2403" t="s">
-        <v>5503</v>
-      </c>
-      <c r="G2403">
-        <v>0</v>
-      </c>
-      <c r="H2403">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2404" spans="1:8">
-      <c r="A2404">
-        <v>2403</v>
-      </c>
-      <c r="B2404">
-        <v>1</v>
-      </c>
-      <c r="C2404">
-        <v>7</v>
-      </c>
-      <c r="D2404" t="s">
-        <v>5506</v>
-      </c>
-      <c r="E2404" t="s">
-        <v>5505</v>
-      </c>
-      <c r="F2404" t="s">
-        <v>5507</v>
-      </c>
-      <c r="G2404">
-        <v>0</v>
-      </c>
-      <c r="H2404">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2405" spans="1:8">
-      <c r="A2405">
-        <v>2404</v>
-      </c>
-      <c r="B2405">
-        <v>1</v>
-      </c>
-      <c r="C2405">
-        <v>7</v>
-      </c>
-      <c r="D2405" t="s">
-        <v>5508</v>
-      </c>
-      <c r="E2405" t="s">
-        <v>5509</v>
-      </c>
-      <c r="F2405" t="s">
-        <v>5510</v>
-      </c>
-      <c r="G2405">
-        <v>0</v>
-      </c>
-      <c r="H2405">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2406" spans="1:8">
-      <c r="A2406">
-        <v>2405</v>
-      </c>
-      <c r="B2406">
-        <v>1</v>
-      </c>
-      <c r="C2406">
-        <v>7</v>
-      </c>
-      <c r="D2406" t="s">
-        <v>2483</v>
-      </c>
-      <c r="E2406" t="s">
-        <v>5511</v>
-      </c>
-      <c r="F2406" t="s">
-        <v>5510</v>
-      </c>
-      <c r="G2406">
-        <v>0</v>
-      </c>
-      <c r="H2406">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2407" spans="1:8">
-      <c r="A2407">
-        <v>2406</v>
-      </c>
-      <c r="B2407">
-        <v>1</v>
-      </c>
-      <c r="C2407">
-        <v>7</v>
-      </c>
-      <c r="D2407" t="s">
-        <v>5512</v>
-      </c>
-      <c r="E2407" t="s">
-        <v>5510</v>
-      </c>
-      <c r="F2407" t="s">
-        <v>5513</v>
-      </c>
-      <c r="G2407">
-        <v>0</v>
-      </c>
-      <c r="H2407">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2408" spans="1:8">
-      <c r="A2408">
-        <v>2407</v>
-      </c>
-      <c r="B2408">
-        <v>1</v>
-      </c>
-      <c r="C2408">
-        <v>7</v>
-      </c>
-      <c r="D2408" t="s">
-        <v>5514</v>
-      </c>
-      <c r="E2408" t="s">
-        <v>5515</v>
-      </c>
-      <c r="F2408" t="s">
-        <v>5516</v>
-      </c>
-      <c r="G2408">
-        <v>0</v>
-      </c>
-      <c r="H2408">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2409" spans="1:8">
-      <c r="A2409">
-        <v>2408</v>
-      </c>
-      <c r="B2409">
-        <v>1</v>
-      </c>
-      <c r="C2409">
-        <v>7</v>
-      </c>
-      <c r="D2409" t="s">
-        <v>5517</v>
-      </c>
-      <c r="E2409" t="s">
-        <v>5515</v>
-      </c>
-      <c r="F2409" t="s">
-        <v>5516</v>
-      </c>
-      <c r="G2409">
-        <v>0</v>
-      </c>
-      <c r="H2409">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2410" spans="1:8">
-      <c r="A2410">
-        <v>2409</v>
-      </c>
-      <c r="B2410">
-        <v>1</v>
-      </c>
-      <c r="C2410">
-        <v>7</v>
-      </c>
-      <c r="D2410" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E2410" t="s">
-        <v>5518</v>
-      </c>
-      <c r="F2410" t="s">
-        <v>5519</v>
-      </c>
-      <c r="G2410">
-        <v>0</v>
-      </c>
-      <c r="H2410">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2411" spans="1:8">
-      <c r="A2411">
-        <v>2410</v>
-      </c>
-      <c r="B2411">
-        <v>1</v>
-      </c>
-      <c r="C2411">
-        <v>7</v>
-      </c>
-      <c r="D2411" t="s">
-        <v>5235</v>
-      </c>
-      <c r="E2411" t="s">
-        <v>5516</v>
-      </c>
-      <c r="F2411" t="s">
-        <v>5520</v>
-      </c>
-      <c r="G2411">
-        <v>0</v>
-      </c>
-      <c r="H2411">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2412" spans="1:8">
-      <c r="A2412">
-        <v>2411</v>
-      </c>
-      <c r="B2412">
-        <v>1</v>
-      </c>
-      <c r="C2412">
-        <v>7</v>
-      </c>
-      <c r="D2412" t="s">
-        <v>5521</v>
-      </c>
-      <c r="E2412" t="s">
-        <v>5522</v>
-      </c>
-      <c r="F2412" t="s">
-        <v>5523</v>
-      </c>
-      <c r="G2412">
-        <v>0</v>
-      </c>
-      <c r="H2412">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2413" spans="1:8">
-      <c r="A2413">
-        <v>2412</v>
-      </c>
-      <c r="B2413">
-        <v>1</v>
-      </c>
-      <c r="C2413">
-        <v>7</v>
-      </c>
-      <c r="D2413" t="s">
-        <v>252</v>
-      </c>
-      <c r="E2413" t="s">
-        <v>5524</v>
-      </c>
-      <c r="F2413" t="s">
-        <v>5525</v>
-      </c>
-      <c r="G2413">
-        <v>0</v>
-      </c>
-      <c r="H2413">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2414" spans="1:8">
-      <c r="A2414">
-        <v>2413</v>
-      </c>
-      <c r="B2414">
-        <v>1</v>
-      </c>
-      <c r="C2414">
-        <v>7</v>
-      </c>
-      <c r="D2414" t="s">
-        <v>5526</v>
-      </c>
-      <c r="E2414" t="s">
-        <v>5527</v>
-      </c>
-      <c r="F2414" t="s">
-        <v>5528</v>
-      </c>
-      <c r="G2414">
-        <v>0</v>
-      </c>
-      <c r="H2414">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2415" spans="1:8">
-      <c r="A2415">
-        <v>2414</v>
-      </c>
-      <c r="B2415">
-        <v>1</v>
-      </c>
-      <c r="C2415">
-        <v>7</v>
-      </c>
-      <c r="D2415" t="s">
-        <v>5529</v>
-      </c>
-      <c r="E2415" t="s">
-        <v>5527</v>
-      </c>
-      <c r="F2415" t="s">
-        <v>5530</v>
-      </c>
-      <c r="G2415">
-        <v>0</v>
-      </c>
-      <c r="H2415">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2416" spans="1:8">
-      <c r="A2416">
-        <v>2415</v>
-      </c>
-      <c r="B2416">
-        <v>1</v>
-      </c>
-      <c r="C2416">
-        <v>7</v>
-      </c>
-      <c r="D2416" t="s">
-        <v>5531</v>
-      </c>
-      <c r="E2416" t="s">
-        <v>5532</v>
-      </c>
-      <c r="F2416" t="s">
-        <v>5533</v>
-      </c>
-      <c r="G2416">
-        <v>0</v>
-      </c>
-      <c r="H2416">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2417" spans="1:8">
-      <c r="A2417">
-        <v>2416</v>
-      </c>
-      <c r="B2417">
-        <v>1</v>
-      </c>
-      <c r="C2417">
-        <v>7</v>
-      </c>
-      <c r="D2417" t="s">
-        <v>759</v>
-      </c>
-      <c r="E2417" t="s">
-        <v>5532</v>
-      </c>
-      <c r="F2417" t="s">
-        <v>5534</v>
-      </c>
-      <c r="G2417">
-        <v>0</v>
-      </c>
-      <c r="H2417">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2418" spans="1:8">
-      <c r="A2418">
-        <v>2417</v>
-      </c>
-      <c r="B2418">
-        <v>1</v>
-      </c>
-      <c r="C2418">
-        <v>7</v>
-      </c>
-      <c r="D2418" t="s">
-        <v>4421</v>
-      </c>
-      <c r="E2418" t="s">
-        <v>5535</v>
-      </c>
-      <c r="F2418" t="s">
-        <v>5536</v>
-      </c>
-      <c r="G2418">
-        <v>0</v>
-      </c>
-      <c r="H2418">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2419" spans="1:8">
-      <c r="A2419">
-        <v>2418</v>
-      </c>
-      <c r="B2419">
-        <v>1</v>
-      </c>
-      <c r="C2419">
-        <v>7</v>
-      </c>
-      <c r="D2419" t="s">
-        <v>837</v>
-      </c>
-      <c r="E2419" t="s">
-        <v>5537</v>
-      </c>
-      <c r="F2419" t="s">
-        <v>5538</v>
-      </c>
-      <c r="G2419">
-        <v>0</v>
-      </c>
-      <c r="H2419">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2420" spans="1:8">
-      <c r="A2420">
-        <v>2419</v>
-      </c>
-      <c r="B2420">
-        <v>1</v>
-      </c>
-      <c r="C2420">
-        <v>7</v>
-      </c>
-      <c r="D2420" t="s">
-        <v>5539</v>
-      </c>
-      <c r="E2420" t="s">
-        <v>5540</v>
-      </c>
-      <c r="F2420" t="s">
-        <v>5541</v>
-      </c>
-      <c r="G2420">
-        <v>0</v>
-      </c>
-      <c r="H2420">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2421" spans="1:8">
-      <c r="A2421">
-        <v>2420</v>
-      </c>
-      <c r="B2421">
-        <v>1</v>
-      </c>
-      <c r="C2421">
-        <v>7</v>
-      </c>
-      <c r="D2421" t="s">
-        <v>5542</v>
-      </c>
-      <c r="E2421" t="s">
-        <v>5540</v>
-      </c>
-      <c r="F2421" t="s">
-        <v>5543</v>
-      </c>
-      <c r="G2421">
-        <v>0</v>
-      </c>
-      <c r="H2421">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2422" spans="1:8">
-      <c r="A2422">
-        <v>2421</v>
-      </c>
-      <c r="B2422">
-        <v>1</v>
-      </c>
-      <c r="C2422">
-        <v>7</v>
-      </c>
-      <c r="D2422" t="s">
-        <v>5544</v>
-      </c>
-      <c r="E2422" t="s">
-        <v>5540</v>
-      </c>
-      <c r="F2422" t="s">
-        <v>5543</v>
-      </c>
-      <c r="G2422">
-        <v>0</v>
-      </c>
-      <c r="H2422">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2423" spans="1:8">
-      <c r="A2423">
-        <v>2422</v>
-      </c>
-      <c r="B2423">
-        <v>1</v>
-      </c>
-      <c r="C2423">
-        <v>7</v>
-      </c>
-      <c r="D2423" t="s">
-        <v>5485</v>
-      </c>
-      <c r="E2423" t="s">
-        <v>5545</v>
-      </c>
-      <c r="F2423" t="s">
-        <v>5546</v>
-      </c>
-      <c r="G2423">
-        <v>0</v>
-      </c>
-      <c r="H2423">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2424" spans="1:8">
-      <c r="A2424">
-        <v>2423</v>
-      </c>
-      <c r="B2424">
-        <v>1</v>
-      </c>
-      <c r="C2424">
-        <v>7</v>
-      </c>
-      <c r="D2424" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2424" t="s">
-        <v>5547</v>
-      </c>
-      <c r="F2424" t="s">
-        <v>5546</v>
-      </c>
-      <c r="G2424">
-        <v>0</v>
-      </c>
-      <c r="H2424">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2425" spans="1:8">
-      <c r="A2425">
-        <v>2424</v>
-      </c>
-      <c r="B2425">
-        <v>1</v>
-      </c>
-      <c r="C2425">
-        <v>7</v>
-      </c>
-      <c r="D2425" t="s">
-        <v>5548</v>
-      </c>
-      <c r="E2425" t="s">
-        <v>5549</v>
-      </c>
-      <c r="F2425" t="s">
-        <v>5550</v>
-      </c>
-      <c r="G2425">
-        <v>0</v>
-      </c>
-      <c r="H2425">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2426" spans="1:8">
-      <c r="A2426">
-        <v>2425</v>
-      </c>
-      <c r="B2426">
-        <v>1</v>
-      </c>
-      <c r="C2426">
-        <v>7</v>
-      </c>
-      <c r="D2426" t="s">
-        <v>5551</v>
-      </c>
-      <c r="E2426" t="s">
-        <v>5552</v>
-      </c>
-      <c r="F2426" t="s">
-        <v>5553</v>
-      </c>
-      <c r="G2426">
-        <v>0</v>
-      </c>
-      <c r="H2426">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2427" spans="1:8">
-      <c r="A2427">
-        <v>2426</v>
-      </c>
-      <c r="B2427">
-        <v>1</v>
-      </c>
-      <c r="C2427">
-        <v>7</v>
-      </c>
-      <c r="D2427" t="s">
-        <v>5554</v>
-      </c>
-      <c r="E2427" t="s">
-        <v>5555</v>
-      </c>
-      <c r="F2427" t="s">
-        <v>5556</v>
-      </c>
-      <c r="G2427">
-        <v>0</v>
-      </c>
-      <c r="H2427">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2428" spans="1:8">
-      <c r="A2428">
-        <v>2427</v>
-      </c>
-      <c r="B2428">
-        <v>1</v>
-      </c>
-      <c r="C2428">
-        <v>7</v>
-      </c>
-      <c r="D2428" t="s">
-        <v>5554</v>
-      </c>
-      <c r="E2428" t="s">
-        <v>5557</v>
-      </c>
-      <c r="F2428" t="s">
-        <v>5558</v>
-      </c>
-      <c r="G2428">
-        <v>0</v>
-      </c>
-      <c r="H2428">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2429" spans="1:8">
-      <c r="A2429">
-        <v>2428</v>
-      </c>
-      <c r="B2429">
-        <v>1</v>
-      </c>
-      <c r="C2429">
-        <v>7</v>
-      </c>
-      <c r="D2429" t="s">
-        <v>5559</v>
-      </c>
-      <c r="E2429" t="s">
-        <v>5560</v>
-      </c>
-      <c r="F2429" t="s">
-        <v>5561</v>
-      </c>
-      <c r="G2429">
-        <v>0</v>
-      </c>
-      <c r="H2429">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2430" spans="1:8">
-      <c r="A2430">
-        <v>2429</v>
-      </c>
-      <c r="B2430">
-        <v>1</v>
-      </c>
-      <c r="C2430">
-        <v>7</v>
-      </c>
-      <c r="D2430" t="s">
-        <v>2473</v>
-      </c>
-      <c r="E2430" t="s">
-        <v>5560</v>
-      </c>
-      <c r="F2430" t="s">
-        <v>5561</v>
-      </c>
-      <c r="G2430">
-        <v>0</v>
-      </c>
-      <c r="H2430">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2431" spans="1:8">
-      <c r="A2431">
-        <v>2430</v>
-      </c>
-      <c r="B2431">
-        <v>1</v>
-      </c>
-      <c r="C2431">
-        <v>7</v>
-      </c>
-      <c r="D2431" t="s">
-        <v>4434</v>
-      </c>
-      <c r="E2431" t="s">
-        <v>5562</v>
-      </c>
-      <c r="F2431" t="s">
-        <v>5563</v>
-      </c>
-      <c r="G2431">
-        <v>0</v>
-      </c>
-      <c r="H2431">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2432" spans="1:8">
-      <c r="A2432">
-        <v>2431</v>
-      </c>
-      <c r="B2432">
-        <v>1</v>
-      </c>
-      <c r="C2432">
-        <v>7</v>
-      </c>
-      <c r="D2432" t="s">
-        <v>5564</v>
-      </c>
-      <c r="E2432" t="s">
-        <v>5565</v>
-      </c>
-      <c r="F2432" t="s">
-        <v>5566</v>
-      </c>
-      <c r="G2432">
-        <v>0</v>
-      </c>
-      <c r="H2432">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2433" spans="1:8">
-      <c r="A2433">
-        <v>2432</v>
-      </c>
-      <c r="B2433">
-        <v>1</v>
-      </c>
-      <c r="C2433">
-        <v>7</v>
-      </c>
-      <c r="D2433" t="s">
-        <v>855</v>
-      </c>
-      <c r="E2433" t="s">
-        <v>5567</v>
-      </c>
-      <c r="F2433" t="s">
-        <v>5568</v>
-      </c>
-      <c r="G2433">
-        <v>0</v>
-      </c>
-      <c r="H2433">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2434" spans="1:8">
-      <c r="A2434">
-        <v>2433</v>
-      </c>
-      <c r="B2434">
-        <v>1</v>
-      </c>
-      <c r="C2434">
-        <v>7</v>
-      </c>
-      <c r="D2434" t="s">
-        <v>5569</v>
-      </c>
-      <c r="E2434" t="s">
-        <v>5570</v>
-      </c>
-      <c r="F2434" t="s">
-        <v>5571</v>
-      </c>
-      <c r="G2434">
-        <v>0</v>
-      </c>
-      <c r="H2434">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2435" spans="1:8">
-      <c r="A2435">
-        <v>2434</v>
-      </c>
-      <c r="B2435">
-        <v>1</v>
-      </c>
-      <c r="C2435">
-        <v>7</v>
-      </c>
-      <c r="D2435" t="s">
-        <v>5572</v>
-      </c>
-      <c r="E2435" t="s">
-        <v>5573</v>
-      </c>
-      <c r="F2435" t="s">
-        <v>5571</v>
-      </c>
-      <c r="G2435">
-        <v>0</v>
-      </c>
-      <c r="H2435">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2436" spans="1:8">
-      <c r="A2436">
-        <v>2435</v>
-      </c>
-      <c r="B2436">
-        <v>1</v>
-      </c>
-      <c r="C2436">
-        <v>7</v>
-      </c>
-      <c r="D2436" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2436" t="s">
-        <v>5574</v>
-      </c>
-      <c r="F2436" t="s">
-        <v>5575</v>
-      </c>
-      <c r="G2436">
-        <v>0</v>
-      </c>
-      <c r="H2436">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2437" spans="1:8">
-      <c r="A2437">
-        <v>2436</v>
-      </c>
-      <c r="B2437">
-        <v>1</v>
-      </c>
-      <c r="C2437">
-        <v>7</v>
-      </c>
-      <c r="D2437" t="s">
-        <v>5578</v>
-      </c>
-      <c r="E2437" t="s">
-        <v>5576</v>
-      </c>
-      <c r="F2437" t="s">
-        <v>5577</v>
-      </c>
-      <c r="G2437">
-        <v>0</v>
-      </c>
-      <c r="H2437">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2438" spans="1:8">
-      <c r="A2438">
-        <v>2437</v>
-      </c>
-      <c r="B2438">
-        <v>1</v>
-      </c>
-      <c r="C2438">
-        <v>7</v>
-      </c>
-      <c r="D2438" t="s">
-        <v>5579</v>
-      </c>
-      <c r="E2438" t="s">
-        <v>5580</v>
-      </c>
-      <c r="F2438" t="s">
-        <v>5577</v>
-      </c>
-      <c r="G2438">
-        <v>0</v>
-      </c>
-      <c r="H2438">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2439" spans="1:8">
-      <c r="A2439">
-        <v>2438</v>
-      </c>
-      <c r="B2439">
-        <v>1</v>
-      </c>
-      <c r="C2439">
-        <v>7</v>
-      </c>
-      <c r="D2439" t="s">
-        <v>5581</v>
-      </c>
-      <c r="E2439" t="s">
-        <v>5582</v>
-      </c>
-      <c r="F2439" t="s">
-        <v>5583</v>
-      </c>
-      <c r="G2439">
-        <v>0</v>
-      </c>
-      <c r="H2439">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2440" spans="1:8">
-      <c r="A2440">
-        <v>2439</v>
-      </c>
-      <c r="B2440">
-        <v>1</v>
-      </c>
-      <c r="C2440">
-        <v>7</v>
-      </c>
-      <c r="D2440" t="s">
-        <v>2651</v>
-      </c>
-      <c r="E2440" t="s">
-        <v>5584</v>
-      </c>
-      <c r="F2440" t="s">
-        <v>5583</v>
-      </c>
-      <c r="G2440">
-        <v>0</v>
-      </c>
-      <c r="H2440">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2441" spans="1:8">
-      <c r="A2441">
-        <v>2440</v>
-      </c>
-      <c r="B2441">
-        <v>1</v>
-      </c>
-      <c r="C2441">
-        <v>7</v>
-      </c>
-      <c r="D2441" t="s">
-        <v>5585</v>
-      </c>
-      <c r="E2441" t="s">
-        <v>5586</v>
-      </c>
-      <c r="F2441" t="s">
-        <v>5587</v>
-      </c>
-      <c r="G2441">
-        <v>0</v>
-      </c>
-      <c r="H2441">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2442" spans="1:8">
-      <c r="A2442">
-        <v>2441</v>
-      </c>
-      <c r="B2442">
-        <v>1</v>
-      </c>
-      <c r="C2442">
-        <v>7</v>
-      </c>
-      <c r="D2442" t="s">
-        <v>5588</v>
-      </c>
-      <c r="E2442" t="s">
-        <v>5589</v>
-      </c>
-      <c r="F2442" t="s">
-        <v>5590</v>
-      </c>
-      <c r="G2442">
-        <v>0</v>
-      </c>
-      <c r="H2442">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2443" spans="1:8">
-      <c r="A2443">
-        <v>2442</v>
-      </c>
-      <c r="B2443">
-        <v>1</v>
-      </c>
-      <c r="C2443">
-        <v>7</v>
-      </c>
-      <c r="D2443" t="s">
-        <v>5591</v>
-      </c>
-      <c r="E2443" t="s">
-        <v>5592</v>
-      </c>
-      <c r="F2443" t="s">
-        <v>5593</v>
-      </c>
-      <c r="G2443">
-        <v>0</v>
-      </c>
-      <c r="H2443">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2444" spans="1:8">
-      <c r="A2444">
-        <v>2443</v>
-      </c>
-      <c r="B2444">
-        <v>1</v>
-      </c>
-      <c r="C2444">
-        <v>7</v>
-      </c>
-      <c r="D2444" t="s">
-        <v>5594</v>
-      </c>
-      <c r="E2444" t="s">
-        <v>5590</v>
-      </c>
-      <c r="F2444" t="s">
-        <v>5595</v>
-      </c>
-      <c r="G2444">
-        <v>0</v>
-      </c>
-      <c r="H2444">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2445" spans="1:8">
-      <c r="A2445">
-        <v>2444</v>
-      </c>
-      <c r="B2445">
-        <v>1</v>
-      </c>
-      <c r="C2445">
-        <v>7</v>
-      </c>
-      <c r="D2445" t="s">
-        <v>3824</v>
-      </c>
-      <c r="E2445" t="s">
-        <v>5596</v>
-      </c>
-      <c r="F2445" t="s">
-        <v>5597</v>
-      </c>
-      <c r="G2445">
-        <v>0</v>
-      </c>
-      <c r="H2445">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2446" spans="1:8">
-      <c r="A2446">
-        <v>2445</v>
-      </c>
-      <c r="B2446">
-        <v>1</v>
-      </c>
-      <c r="C2446">
-        <v>7</v>
-      </c>
-      <c r="D2446" t="s">
-        <v>5598</v>
-      </c>
-      <c r="E2446" t="s">
-        <v>5599</v>
-      </c>
-      <c r="F2446" t="s">
-        <v>5600</v>
-      </c>
-      <c r="G2446">
-        <v>0</v>
-      </c>
-      <c r="H2446">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2447" spans="1:8">
-      <c r="A2447">
-        <v>2446</v>
-      </c>
-      <c r="B2447">
-        <v>1</v>
-      </c>
-      <c r="C2447">
-        <v>7</v>
-      </c>
-      <c r="D2447" t="s">
-        <v>5601</v>
-      </c>
-      <c r="E2447" t="s">
-        <v>5602</v>
-      </c>
-      <c r="F2447" t="s">
-        <v>5603</v>
-      </c>
-      <c r="G2447">
-        <v>0</v>
-      </c>
-      <c r="H2447">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2448" spans="1:8">
-      <c r="A2448">
-        <v>2447</v>
-      </c>
-      <c r="B2448">
-        <v>1</v>
-      </c>
-      <c r="C2448">
-        <v>7</v>
-      </c>
-      <c r="D2448" t="s">
-        <v>966</v>
-      </c>
-      <c r="E2448" t="s">
-        <v>5604</v>
-      </c>
-      <c r="F2448" t="s">
-        <v>5605</v>
-      </c>
-      <c r="G2448">
-        <v>0</v>
-      </c>
-      <c r="H2448">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2449" spans="1:8">
-      <c r="A2449">
-        <v>2448</v>
-      </c>
-      <c r="B2449">
-        <v>1</v>
-      </c>
-      <c r="C2449">
-        <v>7</v>
-      </c>
-      <c r="D2449" t="s">
-        <v>5606</v>
-      </c>
-      <c r="E2449" t="s">
-        <v>5607</v>
-      </c>
-      <c r="F2449" t="s">
-        <v>5608</v>
-      </c>
-      <c r="G2449">
-        <v>0</v>
-      </c>
-      <c r="H2449">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2450" spans="1:8">
-      <c r="A2450">
-        <v>2449</v>
-      </c>
-      <c r="B2450">
-        <v>1</v>
-      </c>
-      <c r="C2450">
-        <v>7</v>
-      </c>
-      <c r="D2450" t="s">
-        <v>5609</v>
-      </c>
-      <c r="E2450" t="s">
-        <v>5610</v>
-      </c>
-      <c r="F2450" t="s">
-        <v>5611</v>
-      </c>
-      <c r="G2450">
-        <v>0</v>
-      </c>
-      <c r="H2450">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2451" spans="1:8">
-      <c r="A2451">
-        <v>2450</v>
-      </c>
-      <c r="B2451">
-        <v>1</v>
-      </c>
-      <c r="C2451">
-        <v>7</v>
-      </c>
-      <c r="D2451" t="s">
-        <v>5612</v>
-      </c>
-      <c r="E2451" t="s">
-        <v>5613</v>
-      </c>
-      <c r="F2451" t="s">
-        <v>5614</v>
-      </c>
-      <c r="G2451">
-        <v>0</v>
-      </c>
-      <c r="H2451">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2452" spans="1:8">
-      <c r="A2452">
-        <v>2451</v>
-      </c>
-      <c r="B2452">
-        <v>1</v>
-      </c>
-      <c r="C2452">
-        <v>7</v>
-      </c>
-      <c r="D2452" t="s">
-        <v>5615</v>
-      </c>
-      <c r="E2452" t="s">
-        <v>5616</v>
-      </c>
-      <c r="F2452" t="s">
-        <v>5617</v>
-      </c>
-      <c r="G2452">
-        <v>0</v>
-      </c>
-      <c r="H2452">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2453" spans="1:8">
-      <c r="A2453">
-        <v>2452</v>
-      </c>
-      <c r="B2453">
-        <v>1</v>
-      </c>
-      <c r="C2453">
-        <v>7</v>
-      </c>
-      <c r="D2453" t="s">
-        <v>5618</v>
-      </c>
-      <c r="E2453" t="s">
-        <v>5611</v>
-      </c>
-      <c r="F2453" t="s">
-        <v>5619</v>
-      </c>
-      <c r="G2453">
-        <v>0</v>
-      </c>
-      <c r="H2453">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2454" spans="1:8">
-      <c r="A2454">
-        <v>2453</v>
-      </c>
-      <c r="B2454">
-        <v>1</v>
-      </c>
-      <c r="C2454">
-        <v>7</v>
-      </c>
-      <c r="D2454" t="s">
-        <v>5620</v>
-      </c>
-      <c r="E2454" t="s">
-        <v>5614</v>
-      </c>
-      <c r="F2454" t="s">
-        <v>5619</v>
-      </c>
-      <c r="G2454">
-        <v>0</v>
-      </c>
-      <c r="H2454">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2455" spans="1:8">
-      <c r="A2455">
-        <v>2454</v>
-      </c>
-      <c r="B2455">
-        <v>1</v>
-      </c>
-      <c r="C2455">
-        <v>7</v>
-      </c>
-      <c r="D2455" t="s">
-        <v>2566</v>
-      </c>
-      <c r="E2455" t="s">
-        <v>5621</v>
-      </c>
-      <c r="F2455" t="s">
-        <v>5622</v>
-      </c>
-      <c r="G2455">
-        <v>0</v>
-      </c>
-      <c r="H2455">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2456" spans="1:8">
-      <c r="A2456">
-        <v>2455</v>
-      </c>
-      <c r="B2456">
-        <v>1</v>
-      </c>
-      <c r="C2456">
-        <v>7</v>
-      </c>
-      <c r="D2456" t="s">
-        <v>5623</v>
-      </c>
-      <c r="E2456" t="s">
-        <v>5621</v>
-      </c>
-      <c r="F2456" t="s">
-        <v>5624</v>
-      </c>
-      <c r="G2456">
-        <v>0</v>
-      </c>
-      <c r="H2456">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2457" spans="1:8">
-      <c r="A2457">
-        <v>2456</v>
-      </c>
-      <c r="B2457">
-        <v>1</v>
-      </c>
-      <c r="C2457">
-        <v>7</v>
-      </c>
-      <c r="D2457" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E2457" t="s">
-        <v>5625</v>
-      </c>
-      <c r="F2457" t="s">
-        <v>5626</v>
-      </c>
-      <c r="G2457">
-        <v>0</v>
-      </c>
-      <c r="H2457">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2458" spans="1:8">
-      <c r="A2458">
-        <v>2457</v>
-      </c>
-      <c r="B2458">
-        <v>1</v>
-      </c>
-      <c r="C2458">
-        <v>7</v>
-      </c>
-      <c r="D2458" t="s">
-        <v>5627</v>
-      </c>
-      <c r="E2458" t="s">
-        <v>5628</v>
-      </c>
-      <c r="F2458" t="s">
-        <v>5629</v>
-      </c>
-      <c r="G2458">
-        <v>0</v>
-      </c>
-      <c r="H2458">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2459" spans="1:8">
-      <c r="A2459">
-        <v>2458</v>
-      </c>
-      <c r="B2459">
-        <v>1</v>
-      </c>
-      <c r="C2459">
-        <v>7</v>
-      </c>
-      <c r="D2459" t="s">
-        <v>474</v>
-      </c>
-      <c r="E2459" t="s">
-        <v>5628</v>
-      </c>
-      <c r="F2459" t="s">
-        <v>5630</v>
-      </c>
-      <c r="G2459">
-        <v>0</v>
-      </c>
-      <c r="H2459">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2460" spans="1:8">
-      <c r="A2460">
-        <v>2459</v>
-      </c>
-      <c r="B2460">
-        <v>1</v>
-      </c>
-      <c r="C2460">
-        <v>7</v>
-      </c>
-      <c r="D2460" t="s">
-        <v>5631</v>
-      </c>
-      <c r="E2460" t="s">
-        <v>5632</v>
-      </c>
-      <c r="F2460" t="s">
-        <v>5633</v>
-      </c>
-      <c r="G2460">
-        <v>0</v>
-      </c>
-      <c r="H2460">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2461" spans="1:8">
-      <c r="A2461">
-        <v>2460</v>
-      </c>
-      <c r="B2461">
-        <v>1</v>
-      </c>
-      <c r="C2461">
-        <v>7</v>
-      </c>
-      <c r="D2461" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E2461" t="s">
-        <v>5634</v>
-      </c>
-      <c r="F2461" t="s">
-        <v>5635</v>
-      </c>
-      <c r="G2461">
-        <v>0</v>
-      </c>
-      <c r="H2461">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2462" spans="1:8">
-      <c r="A2462">
-        <v>2461</v>
-      </c>
-      <c r="B2462">
-        <v>1</v>
-      </c>
-      <c r="C2462">
-        <v>7</v>
-      </c>
-      <c r="D2462" t="s">
-        <v>3315</v>
-      </c>
-      <c r="E2462" t="s">
-        <v>5636</v>
-      </c>
-      <c r="F2462" t="s">
-        <v>5637</v>
-      </c>
-      <c r="G2462">
-        <v>0</v>
-      </c>
-      <c r="H2462">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2463" spans="1:8">
-      <c r="A2463">
-        <v>2462</v>
-      </c>
-      <c r="B2463">
-        <v>1</v>
-      </c>
-      <c r="C2463">
-        <v>7</v>
-      </c>
-      <c r="D2463" t="s">
-        <v>5638</v>
-      </c>
-      <c r="E2463" t="s">
-        <v>5639</v>
-      </c>
-      <c r="F2463" t="s">
-        <v>5640</v>
-      </c>
-      <c r="G2463">
-        <v>0</v>
-      </c>
-      <c r="H2463">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2464" spans="1:8">
-      <c r="A2464">
-        <v>2463</v>
-      </c>
-      <c r="B2464">
-        <v>1</v>
-      </c>
-      <c r="C2464">
-        <v>7</v>
-      </c>
-      <c r="D2464" t="s">
-        <v>5641</v>
-      </c>
-      <c r="E2464" t="s">
-        <v>5639</v>
-      </c>
-      <c r="F2464" t="s">
-        <v>5642</v>
-      </c>
-      <c r="G2464">
-        <v>0</v>
-      </c>
-      <c r="H2464">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2465" spans="1:8">
-      <c r="A2465">
-        <v>2464</v>
-      </c>
-      <c r="B2465">
-        <v>1</v>
-      </c>
-      <c r="C2465">
-        <v>7</v>
-      </c>
-      <c r="D2465" t="s">
-        <v>5643</v>
-      </c>
-      <c r="E2465" t="s">
-        <v>5644</v>
-      </c>
-      <c r="F2465" t="s">
-        <v>5645</v>
-      </c>
-      <c r="G2465">
-        <v>0</v>
-      </c>
-      <c r="H2465">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2466" spans="1:8">
-      <c r="A2466">
-        <v>2465</v>
-      </c>
-      <c r="B2466">
-        <v>1</v>
-      </c>
-      <c r="C2466">
-        <v>7</v>
-      </c>
-      <c r="D2466" t="s">
-        <v>3782</v>
-      </c>
-      <c r="E2466" t="s">
-        <v>5646</v>
-      </c>
-      <c r="F2466" t="s">
-        <v>5645</v>
-      </c>
-      <c r="G2466">
-        <v>0</v>
-      </c>
-      <c r="H2466">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2467" spans="1:8">
-      <c r="A2467">
-        <v>2466</v>
-      </c>
-      <c r="B2467">
-        <v>1</v>
-      </c>
-      <c r="C2467">
-        <v>7</v>
-      </c>
-      <c r="D2467" t="s">
-        <v>5647</v>
-      </c>
-      <c r="E2467" t="s">
-        <v>5648</v>
-      </c>
-      <c r="F2467" t="s">
-        <v>5649</v>
-      </c>
-      <c r="G2467">
-        <v>0</v>
-      </c>
-      <c r="H2467">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2468" spans="1:8">
-      <c r="A2468">
-        <v>2467</v>
-      </c>
-      <c r="B2468">
-        <v>1</v>
-      </c>
-      <c r="C2468">
-        <v>7</v>
-      </c>
-      <c r="D2468" t="s">
-        <v>5650</v>
-      </c>
-      <c r="E2468" t="s">
-        <v>5651</v>
-      </c>
-      <c r="F2468" t="s">
-        <v>5652</v>
-      </c>
-      <c r="G2468">
-        <v>0</v>
-      </c>
-      <c r="H2468">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2469" spans="1:8">
-      <c r="A2469">
-        <v>2468</v>
-      </c>
-      <c r="B2469">
-        <v>1</v>
-      </c>
-      <c r="C2469">
-        <v>7</v>
-      </c>
-      <c r="D2469" t="s">
-        <v>3631</v>
-      </c>
-      <c r="E2469" t="s">
-        <v>5653</v>
-      </c>
-      <c r="F2469" t="s">
-        <v>5654</v>
-      </c>
-      <c r="G2469">
-        <v>0</v>
-      </c>
-      <c r="H2469">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2470" spans="1:8">
-      <c r="A2470">
-        <v>2469</v>
-      </c>
-      <c r="B2470">
-        <v>1</v>
-      </c>
-      <c r="C2470">
-        <v>7</v>
-      </c>
-      <c r="D2470" t="s">
-        <v>5655</v>
-      </c>
-      <c r="E2470" t="s">
-        <v>5656</v>
-      </c>
-      <c r="F2470" t="s">
-        <v>5657</v>
-      </c>
-      <c r="G2470">
-        <v>0</v>
-      </c>
-      <c r="H2470">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2471" spans="1:8">
-      <c r="A2471">
-        <v>2470</v>
-      </c>
-      <c r="B2471">
-        <v>1</v>
-      </c>
-      <c r="C2471">
-        <v>7</v>
-      </c>
-      <c r="D2471" t="s">
-        <v>5658</v>
-      </c>
-      <c r="E2471" t="s">
-        <v>5656</v>
-      </c>
-      <c r="F2471" t="s">
-        <v>5659</v>
-      </c>
-      <c r="G2471">
-        <v>0</v>
-      </c>
-      <c r="H2471">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2472" spans="1:8">
-      <c r="A2472">
-        <v>2471</v>
-      </c>
-      <c r="B2472">
-        <v>1</v>
-      </c>
-      <c r="C2472">
-        <v>7</v>
-      </c>
-      <c r="D2472" t="s">
-        <v>5660</v>
-      </c>
-      <c r="E2472" t="s">
-        <v>5661</v>
-      </c>
-      <c r="F2472" t="s">
-        <v>5662</v>
-      </c>
-      <c r="G2472">
-        <v>0</v>
-      </c>
-      <c r="H2472">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2473" spans="1:8">
-      <c r="A2473">
-        <v>2472</v>
-      </c>
-      <c r="B2473">
-        <v>1</v>
-      </c>
-      <c r="C2473">
-        <v>7</v>
-      </c>
-      <c r="D2473" t="s">
-        <v>5663</v>
-      </c>
-      <c r="E2473" t="s">
-        <v>5662</v>
-      </c>
-      <c r="F2473" t="s">
-        <v>5664</v>
-      </c>
-      <c r="G2473">
-        <v>0</v>
-      </c>
-      <c r="H2473">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2474" spans="1:8">
-      <c r="A2474">
-        <v>2473</v>
-      </c>
-      <c r="B2474">
-        <v>1</v>
-      </c>
-      <c r="C2474">
-        <v>7</v>
-      </c>
-      <c r="G2474">
-        <v>0</v>
-      </c>
-      <c r="H2474">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2475" spans="1:8">
-      <c r="A2475">
-        <v>2474</v>
-      </c>
-      <c r="B2475">
-        <v>1</v>
-      </c>
-      <c r="C2475">
-        <v>7</v>
-      </c>
-      <c r="G2475">
-        <v>0</v>
-      </c>
-      <c r="H2475">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2476" spans="1:8">
-      <c r="A2476">
-        <v>2475</v>
-      </c>
-      <c r="B2476">
-        <v>1</v>
-      </c>
-      <c r="C2476">
-        <v>7</v>
-      </c>
-      <c r="G2476">
-        <v>0</v>
-      </c>
-      <c r="H2476">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2477" spans="1:8">
-      <c r="A2477">
-        <v>2476</v>
-      </c>
-      <c r="B2477">
-        <v>1</v>
-      </c>
-      <c r="C2477">
-        <v>7</v>
-      </c>
-      <c r="G2477">
-        <v>0</v>
-      </c>
-      <c r="H2477">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2478" spans="1:8">
-      <c r="A2478">
-        <v>2477</v>
-      </c>
-      <c r="B2478">
-        <v>1</v>
-      </c>
-      <c r="C2478">
-        <v>7</v>
-      </c>
-      <c r="G2478">
-        <v>0</v>
-      </c>
-      <c r="H2478">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2479" spans="1:8">
-      <c r="A2479">
-        <v>2478</v>
-      </c>
-      <c r="B2479">
-        <v>1</v>
-      </c>
-      <c r="C2479">
-        <v>7</v>
-      </c>
-      <c r="G2479">
-        <v>0</v>
-      </c>
-      <c r="H2479">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2480" spans="1:8">
-      <c r="A2480">
-        <v>2479</v>
-      </c>
-      <c r="B2480">
-        <v>1</v>
-      </c>
-      <c r="C2480">
-        <v>7</v>
-      </c>
-      <c r="G2480">
-        <v>0</v>
-      </c>
-      <c r="H2480">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2481" spans="1:8">
-      <c r="A2481">
-        <v>2480</v>
-      </c>
-      <c r="B2481">
-        <v>1</v>
-      </c>
-      <c r="C2481">
-        <v>7</v>
-      </c>
-      <c r="G2481">
-        <v>0</v>
-      </c>
-      <c r="H2481">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2482" spans="1:8">
-      <c r="A2482">
-        <v>2481</v>
-      </c>
-      <c r="B2482">
-        <v>1</v>
-      </c>
-      <c r="C2482">
-        <v>7</v>
-      </c>
-      <c r="G2482">
-        <v>0</v>
-      </c>
-      <c r="H2482">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2483" spans="1:8">
-      <c r="A2483">
-        <v>2482</v>
-      </c>
-      <c r="B2483">
-        <v>1</v>
-      </c>
-      <c r="C2483">
-        <v>7</v>
-      </c>
-      <c r="G2483">
-        <v>0</v>
-      </c>
-      <c r="H2483">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2484" spans="1:8">
-      <c r="A2484">
-        <v>2483</v>
-      </c>
-      <c r="B2484">
-        <v>1</v>
-      </c>
-      <c r="C2484">
-        <v>7</v>
-      </c>
-      <c r="G2484">
-        <v>0</v>
-      </c>
-      <c r="H2484">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2485" spans="1:8">
-      <c r="A2485">
-        <v>2484</v>
-      </c>
-      <c r="B2485">
-        <v>1</v>
-      </c>
-      <c r="C2485">
-        <v>7</v>
-      </c>
-      <c r="G2485">
-        <v>0</v>
-      </c>
-      <c r="H2485">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2486" spans="1:8">
-      <c r="A2486">
-        <v>2485</v>
-      </c>
-      <c r="B2486">
-        <v>1</v>
-      </c>
-      <c r="C2486">
-        <v>7</v>
-      </c>
-      <c r="G2486">
-        <v>0</v>
-      </c>
-      <c r="H2486">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2487" spans="1:8">
-      <c r="A2487">
-        <v>2486</v>
-      </c>
-      <c r="B2487">
-        <v>1</v>
-      </c>
-      <c r="C2487">
-        <v>7</v>
-      </c>
-      <c r="G2487">
-        <v>0</v>
-      </c>
-      <c r="H2487">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2488" spans="1:8">
-      <c r="A2488">
-        <v>2487</v>
-      </c>
-      <c r="B2488">
-        <v>1</v>
-      </c>
-      <c r="C2488">
-        <v>7</v>
-      </c>
-      <c r="G2488">
-        <v>0</v>
-      </c>
-      <c r="H2488">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2489" spans="1:8">
-      <c r="A2489">
-        <v>2488</v>
-      </c>
-      <c r="B2489">
-        <v>1</v>
-      </c>
-      <c r="C2489">
-        <v>7</v>
-      </c>
-      <c r="G2489">
-        <v>0</v>
-      </c>
-      <c r="H2489">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2490" spans="1:8">
-      <c r="A2490">
-        <v>2489</v>
-      </c>
-      <c r="B2490">
-        <v>1</v>
-      </c>
-      <c r="C2490">
-        <v>7</v>
-      </c>
-      <c r="G2490">
-        <v>0</v>
-      </c>
-      <c r="H2490">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2491" spans="1:8">
-      <c r="A2491">
-        <v>2490</v>
-      </c>
-      <c r="B2491">
-        <v>1</v>
-      </c>
-      <c r="C2491">
-        <v>7</v>
-      </c>
-      <c r="G2491">
-        <v>0</v>
-      </c>
-      <c r="H2491">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2492" spans="1:8">
-      <c r="A2492">
-        <v>2491</v>
-      </c>
-      <c r="B2492">
-        <v>1</v>
-      </c>
-      <c r="C2492">
-        <v>7</v>
-      </c>
-      <c r="G2492">
-        <v>0</v>
-      </c>
-      <c r="H2492">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2493" spans="1:8">
-      <c r="A2493">
-        <v>2492</v>
-      </c>
-      <c r="B2493">
-        <v>1</v>
-      </c>
-      <c r="C2493">
-        <v>7</v>
-      </c>
-      <c r="G2493">
-        <v>0</v>
-      </c>
-      <c r="H2493">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2494" spans="1:8">
-      <c r="A2494">
-        <v>2493</v>
-      </c>
-      <c r="B2494">
-        <v>1</v>
-      </c>
-      <c r="C2494">
-        <v>7</v>
-      </c>
-      <c r="G2494">
-        <v>0</v>
-      </c>
-      <c r="H2494">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2495" spans="1:8">
-      <c r="A2495">
-        <v>2494</v>
-      </c>
-      <c r="B2495">
-        <v>1</v>
-      </c>
-      <c r="C2495">
-        <v>7</v>
-      </c>
-      <c r="G2495">
-        <v>0</v>
-      </c>
-      <c r="H2495">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2496" spans="1:8">
-      <c r="A2496">
-        <v>2495</v>
-      </c>
-      <c r="B2496">
-        <v>1</v>
-      </c>
-      <c r="C2496">
-        <v>7</v>
-      </c>
-      <c r="G2496">
-        <v>0</v>
-      </c>
-      <c r="H2496">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2497" spans="1:8">
-      <c r="A2497">
-        <v>2496</v>
-      </c>
-      <c r="B2497">
-        <v>1</v>
-      </c>
-      <c r="C2497">
-        <v>7</v>
-      </c>
-      <c r="G2497">
-        <v>0</v>
-      </c>
-      <c r="H2497">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2498" spans="1:8">
-      <c r="A2498">
-        <v>2497</v>
-      </c>
-      <c r="B2498">
-        <v>1</v>
-      </c>
-      <c r="C2498">
-        <v>7</v>
-      </c>
-      <c r="G2498">
-        <v>0</v>
-      </c>
-      <c r="H2498">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2499" spans="1:8">
-      <c r="A2499">
-        <v>2498</v>
-      </c>
-      <c r="B2499">
-        <v>1</v>
-      </c>
-      <c r="C2499">
-        <v>7</v>
-      </c>
-      <c r="G2499">
-        <v>0</v>
-      </c>
-      <c r="H2499">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2500" spans="1:8">
-      <c r="A2500">
-        <v>2499</v>
-      </c>
-      <c r="B2500">
-        <v>1</v>
-      </c>
-      <c r="C2500">
-        <v>7</v>
-      </c>
-      <c r="G2500">
-        <v>0</v>
-      </c>
-      <c r="H2500">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>